<commit_message>
Data package overview updated
</commit_message>
<xml_diff>
--- a/hardware/DataPackage.xlsx
+++ b/hardware/DataPackage.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\Repos\lora\arduino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\Repos\lora\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21EF4FC-642C-46A1-9EF3-E73F7904AA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110739E0-ED33-4F36-8DFB-3DA1357036AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" activeTab="2" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="30636" yWindow="2316" windowWidth="21252" windowHeight="12636" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
     <sheet name="BatteryVotage" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle1" sheetId="3" r:id="rId3"/>
+    <sheet name="First 2 bytes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -306,19 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -328,6 +316,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -340,9 +343,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1781,10 +1781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FF0E6-8FE4-49E3-812F-B76B934E1ACD}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1872,14 +1872,14 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
@@ -1935,14 +1935,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
@@ -2053,7 +2053,7 @@
         <v>64</v>
       </c>
       <c r="E36" s="3">
-        <f>B33/C36</f>
+        <f>$B$33/C36</f>
         <v>65.333333333333329</v>
       </c>
       <c r="F36" s="5">
@@ -2061,7 +2061,7 @@
         <v>65</v>
       </c>
       <c r="G36">
-        <f>B33-F36*C36</f>
+        <f t="shared" ref="G36:G38" si="0">$B$33-F36*C36</f>
         <v>2</v>
       </c>
     </row>
@@ -2070,56 +2070,118 @@
         <v>2</v>
       </c>
       <c r="B37">
-        <f t="shared" ref="B37:B38" si="0">A37*60</f>
+        <f t="shared" ref="B37:B43" si="1">A37*60</f>
         <v>120</v>
       </c>
       <c r="C37">
         <v>7</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:D38" si="1">2^C37</f>
+        <f t="shared" ref="D37:D42" si="2">2^C37</f>
         <v>128</v>
       </c>
       <c r="E37" s="3">
-        <f>B33/C37</f>
+        <f>$B$33/C37</f>
         <v>56</v>
       </c>
       <c r="F37" s="5">
-        <f t="shared" ref="F37:F38" si="2">ROUNDDOWN(E37,0)</f>
+        <f t="shared" ref="F37:F42" si="3">ROUNDDOWN(E37,0)</f>
         <v>56</v>
       </c>
       <c r="G37">
-        <f>B33-F37*C37</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
-        <v>180</v>
+        <f t="shared" si="1"/>
+        <v>240</v>
       </c>
       <c r="C38">
         <v>8</v>
       </c>
       <c r="D38">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+      <c r="E38" s="3">
+        <f>$B$33/C38</f>
+        <v>49</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39">
         <f t="shared" si="1"/>
-        <v>256</v>
-      </c>
-      <c r="E38" s="3">
-        <f>B33/C38</f>
-        <v>49</v>
-      </c>
-      <c r="F38" s="5">
+        <v>480</v>
+      </c>
+      <c r="C39">
+        <v>9</v>
+      </c>
+      <c r="D39">
         <f t="shared" si="2"/>
-        <v>49</v>
-      </c>
-      <c r="G38">
-        <f>B33-F38*C38</f>
-        <v>0</v>
-      </c>
+        <v>512</v>
+      </c>
+      <c r="E39" s="3">
+        <f>$B$33/C39</f>
+        <v>43.555555555555557</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="G39">
+        <f>$B$33-F39*C39</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>17</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="1"/>
+        <v>1020</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>1024</v>
+      </c>
+      <c r="E40" s="3">
+        <f>$B$33/C40</f>
+        <v>39.200000000000003</v>
+      </c>
+      <c r="F40" s="5">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="G40">
+        <f>$B$33-F40*C40</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E42" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2135,7 +2197,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2251,8 +2313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA1C9C9-9441-4141-A399-61EB92DAC4E4}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2261,315 +2323,321 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
+      <c r="A2" s="8">
         <v>7</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="9">
         <v>6</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="9">
         <v>5</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="9">
         <v>4</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="9">
         <v>3</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="9">
         <v>2</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="9">
         <v>1</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="10">
         <v>0</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="8">
         <v>7</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="9">
         <v>6</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="9">
         <v>5</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="9">
         <v>4</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="9">
         <v>3</v>
       </c>
-      <c r="N2" s="12">
+      <c r="N2" s="8">
         <v>2</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="9">
         <v>1</v>
       </c>
-      <c r="P2" s="14">
+      <c r="P2" s="10">
         <v>0</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="15" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="15" t="s">
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="18" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="8" t="s">
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="S6" s="8"/>
+      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7">
         <v>1</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="7">
         <v>0</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="7">
         <v>0</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="7">
         <v>0</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="7">
         <v>1</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="7">
         <v>1</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="7">
         <v>0</v>
       </c>
-      <c r="P7" s="9">
+      <c r="P7" s="7">
         <v>0</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="R7" s="19" t="s">
+      <c r="R7" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="S7" s="19"/>
+      <c r="S7" s="13"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="8" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8" t="s">
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="8">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="14">
         <v>17</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8">
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14">
         <v>4</v>
       </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="8" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="10">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="12">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -2577,12 +2645,6 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
-    <mergeCell ref="R6:S6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
data package information updated
</commit_message>
<xml_diff>
--- a/hardware/DataPackage.xlsx
+++ b/hardware/DataPackage.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\Repos\lora\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110739E0-ED33-4F36-8DFB-3DA1357036AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2178D9-2B5E-4543-8004-BEDAF788808F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30636" yWindow="2316" windowWidth="21252" windowHeight="12636" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" activeTab="1" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
-    <sheet name="BatteryVotage" sheetId="2" r:id="rId2"/>
-    <sheet name="First 2 bytes" sheetId="3" r:id="rId3"/>
+    <sheet name="Decoding" sheetId="5" r:id="rId2"/>
+    <sheet name="BatteryPairing" sheetId="4" r:id="rId3"/>
+    <sheet name="BatteryVotage" sheetId="2" r:id="rId4"/>
+    <sheet name="old_Decoding" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
-  <si>
-    <t>rest 50 bytes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>minutes of day</t>
   </si>
@@ -77,9 +76,6 @@
     <t>size [bit]</t>
   </si>
   <si>
-    <t>battery level</t>
-  </si>
-  <si>
     <t>inkrement [%]</t>
   </si>
   <si>
@@ -135,6 +131,96 @@
   </si>
   <si>
     <t>BatteryIndex</t>
+  </si>
+  <si>
+    <t>Status bits</t>
+  </si>
+  <si>
+    <t>Messages</t>
+  </si>
+  <si>
+    <t>0 = no error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 = </t>
+  </si>
+  <si>
+    <t>min. Temp [°C]</t>
+  </si>
+  <si>
+    <t>max. Temp [°C]</t>
+  </si>
+  <si>
+    <t>dT [°C]</t>
+  </si>
+  <si>
+    <t>increments [°C]</t>
+  </si>
+  <si>
+    <t>Temperatur</t>
+  </si>
+  <si>
+    <t>Battery level</t>
+  </si>
+  <si>
+    <t>Humidity</t>
+  </si>
+  <si>
+    <t>Spare bits</t>
+  </si>
+  <si>
+    <t>remaining bytes</t>
+  </si>
+  <si>
+    <t>Voltage difference</t>
+  </si>
+  <si>
+    <t>Resistor [Ohm]</t>
+  </si>
+  <si>
+    <t>Current [A]</t>
+  </si>
+  <si>
+    <t>max Current [A]</t>
+  </si>
+  <si>
+    <t>Power [W!</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>1 byte</t>
+  </si>
+  <si>
+    <t>2 byte</t>
+  </si>
+  <si>
+    <t>3 byte</t>
+  </si>
+  <si>
+    <t>4 byte</t>
+  </si>
+  <si>
+    <t>Spare</t>
   </si>
 </sst>
 </file>
@@ -144,7 +230,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +248,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -288,13 +380,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -318,14 +447,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -345,13 +474,157 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1781,10 +2054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FF0E6-8FE4-49E3-812F-B76B934E1ACD}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1793,418 +2066,1550 @@
     <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4">
         <f>B1*8</f>
         <v>408</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4">
         <f>B2-B6</f>
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <f>2^B11</f>
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4">
+        <f>B8-B11</f>
+        <v>397</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B18" s="2">
+        <f>100/(2^B17-1)</f>
+        <v>3.225806451612903</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <f>B13-B17</f>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26">
+        <f>B25-B24</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="2">
+        <f>B26/(2^B23-1)</f>
+        <v>2.2580645161290325</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="4">
+        <f>B19-B23</f>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2">
-        <f>100/(2^B12-1)</f>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="2">
+        <f>100/(2^B32-1)</f>
         <v>14.285714285714286</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="4">
-        <f>B9-B12</f>
-        <v>397</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="4">
+        <f>B28-B32</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="4">
+        <f>B34-B38</f>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>1440</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="3">
+        <f>B39/B47</f>
+        <v>34.636363636363633</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="22">
+        <f>ROUNDDOWN(D46,0)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <f>2^B47</f>
+        <v>2048</v>
+      </c>
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48">
+        <f>B39-D47*B47</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="1">
         <v>5</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="1">
+        <f>2^B54</f>
+        <v>32</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="6">
+        <f>B39-B54</f>
+        <v>376</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57" s="1">
+        <f>B57/8</f>
+        <v>47</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" t="s">
+        <v>19</v>
+      </c>
+      <c r="G59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B60">
+        <f>A60*60</f>
+        <v>60</v>
+      </c>
+      <c r="C60">
+        <v>6</v>
+      </c>
+      <c r="D60">
+        <f>2^C60</f>
+        <v>64</v>
+      </c>
+      <c r="E60" s="3">
+        <f>$B$57/C60</f>
+        <v>62.666666666666664</v>
+      </c>
+      <c r="F60" s="5">
+        <f>ROUNDDOWN(E60,0)</f>
+        <v>62</v>
+      </c>
+      <c r="G60">
+        <f t="shared" ref="G60:G62" si="0">$B$57-F60*C60</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
         <v>2</v>
       </c>
-      <c r="B22">
-        <v>1440</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B61">
+        <f t="shared" ref="B61:B64" si="1">A61*60</f>
+        <v>120</v>
+      </c>
+      <c r="C61">
+        <v>7</v>
+      </c>
+      <c r="D61">
+        <f t="shared" ref="D61:D64" si="2">2^C61</f>
+        <v>128</v>
+      </c>
+      <c r="E61" s="3">
+        <f>$B$57/C61</f>
+        <v>53.714285714285715</v>
+      </c>
+      <c r="F61" s="5">
+        <f t="shared" ref="F61:F64" si="3">ROUNDDOWN(E61,0)</f>
+        <v>53</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62">
         <v>4</v>
       </c>
-      <c r="D22" s="3">
-        <f>B15/B23</f>
-        <v>36.090909090909093</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23">
-        <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="5">
-        <f>ROUNDDOWN(D22,0)</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <f>2^B23</f>
-        <v>2048</v>
-      </c>
-      <c r="C24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24">
-        <f>B15-D23*B23</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="1">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="1">
-        <f>2^B30</f>
-        <v>32</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="6">
-        <f>B15-B30</f>
-        <v>392</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="B62">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="C62">
         <v>8</v>
       </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" t="s">
-        <v>21</v>
-      </c>
-      <c r="G35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36">
-        <f>A36*60</f>
-        <v>60</v>
-      </c>
-      <c r="C36">
-        <v>6</v>
-      </c>
-      <c r="D36">
-        <f>2^C36</f>
-        <v>64</v>
-      </c>
-      <c r="E36" s="3">
-        <f>$B$33/C36</f>
-        <v>65.333333333333329</v>
-      </c>
-      <c r="F36" s="5">
-        <f>ROUNDDOWN(E36,0)</f>
-        <v>65</v>
-      </c>
-      <c r="G36">
-        <f t="shared" ref="G36:G38" si="0">$B$33-F36*C36</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>2</v>
-      </c>
-      <c r="B37">
-        <f t="shared" ref="B37:B43" si="1">A37*60</f>
-        <v>120</v>
-      </c>
-      <c r="C37">
-        <v>7</v>
-      </c>
-      <c r="D37">
-        <f t="shared" ref="D37:D42" si="2">2^C37</f>
-        <v>128</v>
-      </c>
-      <c r="E37" s="3">
-        <f>$B$33/C37</f>
-        <v>56</v>
-      </c>
-      <c r="F37" s="5">
-        <f t="shared" ref="F37:F42" si="3">ROUNDDOWN(E37,0)</f>
-        <v>56</v>
-      </c>
-      <c r="G37">
+      <c r="D62">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+      <c r="E62" s="3">
+        <f>$B$57/C62</f>
+        <v>47</v>
+      </c>
+      <c r="F62" s="5">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="G62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>4</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="1"/>
-        <v>240</v>
-      </c>
-      <c r="C38">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63">
         <v>8</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="2"/>
-        <v>256</v>
-      </c>
-      <c r="E38" s="3">
-        <f>$B$33/C38</f>
-        <v>49</v>
-      </c>
-      <c r="F38" s="5">
-        <f t="shared" si="3"/>
-        <v>49</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>8</v>
-      </c>
-      <c r="B39">
+      <c r="B63">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="C39">
+      <c r="C63">
         <v>9</v>
       </c>
-      <c r="D39">
+      <c r="D63">
         <f t="shared" si="2"/>
         <v>512</v>
       </c>
-      <c r="E39" s="3">
-        <f>$B$33/C39</f>
-        <v>43.555555555555557</v>
-      </c>
-      <c r="F39" s="5">
+      <c r="E63" s="3">
+        <f>$B$57/C63</f>
+        <v>41.777777777777779</v>
+      </c>
+      <c r="F63" s="5">
         <f t="shared" si="3"/>
-        <v>43</v>
-      </c>
-      <c r="G39">
-        <f>$B$33-F39*C39</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40">
+        <v>41</v>
+      </c>
+      <c r="G63">
+        <f>$B$57-F63*C63</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64">
         <v>17</v>
       </c>
-      <c r="B40">
+      <c r="B64">
         <f t="shared" si="1"/>
         <v>1020</v>
       </c>
-      <c r="C40">
+      <c r="C64">
         <v>10</v>
       </c>
-      <c r="D40">
+      <c r="D64">
         <f t="shared" si="2"/>
         <v>1024</v>
       </c>
-      <c r="E40" s="3">
-        <f>$B$33/C40</f>
-        <v>39.200000000000003</v>
-      </c>
-      <c r="F40" s="5">
+      <c r="E64" s="3">
+        <f>$B$57/C64</f>
+        <v>37.6</v>
+      </c>
+      <c r="F64" s="5">
         <f t="shared" si="3"/>
-        <v>39</v>
-      </c>
-      <c r="G40">
-        <f>$B$33-F40*C40</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E42" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="G64">
+        <f>$B$57-F64*C64</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E66" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A51:F51"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8852597E-F5BB-40E1-97DB-5D341DB313BD}">
+  <dimension ref="A1:AF11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="32" width="4.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="27"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9">
+        <v>6</v>
+      </c>
+      <c r="C2" s="9">
+        <v>5</v>
+      </c>
+      <c r="D2" s="9">
+        <v>4</v>
+      </c>
+      <c r="E2" s="9">
+        <v>3</v>
+      </c>
+      <c r="F2" s="9">
+        <v>2</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8">
+        <v>7</v>
+      </c>
+      <c r="J2" s="9">
+        <v>6</v>
+      </c>
+      <c r="K2" s="9">
+        <v>5</v>
+      </c>
+      <c r="L2" s="9">
+        <v>4</v>
+      </c>
+      <c r="M2" s="9">
+        <v>3</v>
+      </c>
+      <c r="N2" s="8">
+        <v>2</v>
+      </c>
+      <c r="O2" s="9">
+        <v>1</v>
+      </c>
+      <c r="P2" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>7</v>
+      </c>
+      <c r="R2" s="9">
+        <v>6</v>
+      </c>
+      <c r="S2" s="10">
+        <v>5</v>
+      </c>
+      <c r="T2" s="8">
+        <v>4</v>
+      </c>
+      <c r="U2" s="9">
+        <v>3</v>
+      </c>
+      <c r="V2" s="9">
+        <v>2</v>
+      </c>
+      <c r="W2" s="9">
+        <v>1</v>
+      </c>
+      <c r="X2" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="8">
+        <v>7</v>
+      </c>
+      <c r="Z2" s="9">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="9">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="10">
+        <v>3</v>
+      </c>
+      <c r="AD2" s="8">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="17"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="R3" s="17"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="29"/>
+      <c r="AB3" s="29"/>
+      <c r="AC3" s="30"/>
+      <c r="AD3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE3" s="29"/>
+      <c r="AF3" s="30"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="Q1:X1"/>
+    <mergeCell ref="Y1:AF1"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="AD3:AF3"/>
+    <mergeCell ref="Y3:AC3"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60375C4-1542-425D-BCAB-95F2E2D7A8CC}">
+  <dimension ref="B1:R13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.88671875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="11" customWidth="1"/>
+    <col min="4" max="9" width="5.5546875" style="11" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" style="11"/>
+    <col min="11" max="11" width="4.77734375" style="11" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" style="11" customWidth="1"/>
+    <col min="13" max="18" width="5.5546875" style="11" customWidth="1"/>
+    <col min="19" max="16384" width="11.5546875" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="K3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="12">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12">
+        <v>5</v>
+      </c>
+      <c r="I4" s="12">
+        <v>10</v>
+      </c>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="N4" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="O4" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="P4" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>5</v>
+      </c>
+      <c r="R4" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="12">
+        <f>$C5/D$4</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="12">
+        <f t="shared" ref="E5:I5" si="0">$C5/E$4</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="H5" s="12">
+        <f t="shared" si="0"/>
+        <v>2E-3</v>
+      </c>
+      <c r="I5" s="12">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="M5" s="12">
+        <f>$C5*D5</f>
+        <v>0.01</v>
+      </c>
+      <c r="N5" s="12">
+        <f t="shared" ref="N5:R5" si="1">$C5*E5</f>
+        <v>1E-3</v>
+      </c>
+      <c r="O5" s="12">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="P5" s="12">
+        <f t="shared" si="1"/>
+        <v>1E-4</v>
+      </c>
+      <c r="Q5" s="12">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="R5" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6" s="23"/>
+      <c r="C6" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="12">
+        <f t="shared" ref="D6:I13" si="2">$C6/D$4</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="12">
+        <f t="shared" si="2"/>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" si="2"/>
+        <v>0.02</v>
+      </c>
+      <c r="H6" s="12">
+        <f t="shared" si="2"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I6" s="12">
+        <f t="shared" si="2"/>
+        <v>2E-3</v>
+      </c>
+      <c r="K6" s="23"/>
+      <c r="L6" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="M6" s="12">
+        <f t="shared" ref="M6:M13" si="3">$C6*D6</f>
+        <v>0.04</v>
+      </c>
+      <c r="N6" s="12">
+        <f t="shared" ref="N6:N13" si="4">$C6*E6</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="O6" s="12">
+        <f t="shared" ref="O6:O13" si="5">$C6*F6</f>
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="P6" s="12">
+        <f t="shared" ref="P6:P13" si="6">$C6*G6</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="Q6" s="12">
+        <f t="shared" ref="Q6:Q13" si="7">$C6*H6</f>
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="R6" s="12">
+        <f t="shared" ref="R6:R13" si="8">$C6*I6</f>
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="23"/>
+      <c r="C7" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E7" s="12">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="G7" s="12">
+        <f t="shared" si="2"/>
+        <v>0.03</v>
+      </c>
+      <c r="H7" s="12">
+        <f t="shared" si="2"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I7" s="12">
+        <f t="shared" si="2"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K7" s="23"/>
+      <c r="L7" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="M7" s="12">
+        <f t="shared" si="3"/>
+        <v>0.09</v>
+      </c>
+      <c r="N7" s="12">
+        <f t="shared" si="4"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="O7" s="12">
+        <f t="shared" si="5"/>
+        <v>1.8E-3</v>
+      </c>
+      <c r="P7" s="12">
+        <f t="shared" si="6"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="Q7" s="12">
+        <f t="shared" si="7"/>
+        <v>1.7999999999999998E-4</v>
+      </c>
+      <c r="R7" s="12">
+        <f t="shared" si="8"/>
+        <v>8.9999999999999992E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="23"/>
+      <c r="C8" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" si="2"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K8" s="23"/>
+      <c r="L8" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="M8" s="12">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="N8" s="12">
+        <f t="shared" si="4"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="O8" s="12">
+        <f t="shared" si="5"/>
+        <v>5.000000000000001E-3</v>
+      </c>
+      <c r="P8" s="12">
+        <f t="shared" si="6"/>
+        <v>2.5000000000000005E-3</v>
+      </c>
+      <c r="Q8" s="12">
+        <f t="shared" si="7"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="R8" s="12">
+        <f t="shared" si="8"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="23"/>
+      <c r="C9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="12">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E9" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="12">
+        <f t="shared" si="2"/>
+        <v>0.02</v>
+      </c>
+      <c r="I9" s="12">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="K9" s="23"/>
+      <c r="L9" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="M9" s="12">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="12">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="O9" s="12">
+        <f t="shared" si="5"/>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="P9" s="12">
+        <f t="shared" si="6"/>
+        <v>1.0000000000000002E-2</v>
+      </c>
+      <c r="Q9" s="12">
+        <f t="shared" si="7"/>
+        <v>2E-3</v>
+      </c>
+      <c r="R9" s="12">
+        <f t="shared" si="8"/>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="23"/>
+      <c r="C10" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="12">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E10" s="12">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="12">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+      <c r="I10" s="12">
+        <f t="shared" si="2"/>
+        <v>0.02</v>
+      </c>
+      <c r="K10" s="23"/>
+      <c r="L10" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="M10" s="12">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="N10" s="12">
+        <f t="shared" si="4"/>
+        <v>0.4</v>
+      </c>
+      <c r="O10" s="12">
+        <f t="shared" si="5"/>
+        <v>8.0000000000000016E-2</v>
+      </c>
+      <c r="P10" s="12">
+        <f t="shared" si="6"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="Q10" s="12">
+        <f t="shared" si="7"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="R10" s="12">
+        <f t="shared" si="8"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="23"/>
+      <c r="C11" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="E11" s="12">
+        <f t="shared" si="2"/>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="G11" s="24">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="H11" s="12">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="I11" s="12">
+        <f t="shared" si="2"/>
+        <v>0.03</v>
+      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="M11" s="12">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="N11" s="12">
+        <f t="shared" si="4"/>
+        <v>0.8999999999999998</v>
+      </c>
+      <c r="O11" s="12">
+        <f t="shared" si="5"/>
+        <v>0.18</v>
+      </c>
+      <c r="P11" s="24">
+        <f t="shared" si="6"/>
+        <v>0.09</v>
+      </c>
+      <c r="Q11" s="12">
+        <f t="shared" si="7"/>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="R11" s="12">
+        <f t="shared" si="8"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="23"/>
+      <c r="C12" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="12">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="12">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="M12" s="12">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="N12" s="12">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="O12" s="12">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="P12" s="12">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+      <c r="Q12" s="12">
+        <f t="shared" si="7"/>
+        <v>0.05</v>
+      </c>
+      <c r="R12" s="12">
+        <f t="shared" si="8"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="23"/>
+      <c r="C13" s="12">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="E13" s="12">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H13" s="12">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="I13" s="12">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="K13" s="23"/>
+      <c r="L13" s="12">
+        <v>1</v>
+      </c>
+      <c r="M13" s="12">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="N13" s="12">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="O13" s="12">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="P13" s="12">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q13" s="12">
+        <f t="shared" si="7"/>
+        <v>0.2</v>
+      </c>
+      <c r="R13" s="12">
+        <f t="shared" si="8"/>
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="M3:R3"/>
+    <mergeCell ref="K5:K13"/>
+    <mergeCell ref="B5:B13"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="K3:L4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D5:I13">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>$E$1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77FA5AC-5DA0-4811-9662-3132B719B7F9}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2309,12 +3714,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA1C9C9-9441-4141-A399-61EB92DAC4E4}">
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:M9"/>
+      <selection activeCell="I3" sqref="I3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2324,7 +3729,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -2400,7 +3805,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -2410,14 +3815,14 @@
       <c r="G3" s="17"/>
       <c r="H3" s="18"/>
       <c r="I3" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J3" s="17"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
       <c r="N3" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O3" s="17"/>
       <c r="P3" s="18"/>
@@ -2477,7 +3882,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
@@ -2488,7 +3893,7 @@
       <c r="P6" s="19"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="S6" s="14"/>
     </row>
@@ -2526,12 +3931,12 @@
         <v>0</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="R7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="S7" s="13"/>
+        <v>26</v>
+      </c>
+      <c r="R7" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="S7" s="21"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
@@ -2543,14 +3948,14 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
       <c r="N8" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
@@ -2598,7 +4003,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
       <c r="N10" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
@@ -2620,24 +4025,18 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="12">
+      <c r="N11" s="20">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -2645,6 +4044,12 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
temperature and humidity sensor readings implemented
</commit_message>
<xml_diff>
--- a/hardware/DataPackage.xlsx
+++ b/hardware/DataPackage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\Repos\lora\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2178D9-2B5E-4543-8004-BEDAF788808F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54C1F69-F480-4D13-A3FC-242BF3636A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" activeTab="1" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="9600" yWindow="2748" windowWidth="21252" windowHeight="12636" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <t>minutes of day</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>Spare</t>
+  </si>
+  <si>
+    <t>Intervall index</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -423,7 +429,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,39 +459,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -505,13 +487,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -519,108 +531,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2054,10 +1964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FF0E6-8FE4-49E3-812F-B76B934E1ACD}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2296,7 +2206,7 @@
         <v>11</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2305,18 +2215,18 @@
       </c>
       <c r="B39" s="4">
         <f>B34-B38</f>
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
@@ -2335,7 +2245,7 @@
       </c>
       <c r="D46" s="3">
         <f>B39/B47</f>
-        <v>34.636363636363633</v>
+        <v>34.909090909090907</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2348,7 +2258,7 @@
       <c r="C47" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D47" s="14">
         <f>ROUNDDOWN(D46,0)</f>
         <v>34</v>
       </c>
@@ -2363,20 +2273,20 @@
       </c>
       <c r="D48">
         <f>B39-D47*B47</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2384,241 +2294,300 @@
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B53" s="1"/>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="13"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B54" s="1">
-        <v>5</v>
+      <c r="B54" s="13">
+        <v>3</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B55" s="1">
-        <f>2^B54</f>
-        <v>32</v>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="32">
+        <f>B39-B54</f>
+        <v>381</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="6">
-        <f>B39-B54</f>
-        <v>376</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D57" s="1">
-        <f>B57/8</f>
-        <v>47</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="1">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1"/>
       <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="1">
+        <f>2^B58</f>
+        <v>32</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" s="6">
+        <f>B55-B58</f>
+        <v>376</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" s="1">
+        <f>B61/8</f>
+        <v>47</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
         <v>9</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C63" t="s">
         <v>7</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D63" t="s">
         <v>5</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E63" t="s">
         <v>6</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F63" t="s">
         <v>3</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G63" t="s">
         <v>19</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H63" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>0</v>
+      </c>
+      <c r="B64">
         <v>1</v>
       </c>
-      <c r="B60">
-        <f>A60*60</f>
+      <c r="C64">
+        <f>B64*60</f>
         <v>60</v>
       </c>
-      <c r="C60">
+      <c r="D64">
         <v>6</v>
       </c>
-      <c r="D60">
-        <f>2^C60</f>
+      <c r="E64">
+        <f>2^D64</f>
         <v>64</v>
       </c>
-      <c r="E60" s="3">
-        <f>$B$57/C60</f>
+      <c r="F64" s="3">
+        <f>$B$61/D64</f>
         <v>62.666666666666664</v>
       </c>
-      <c r="F60" s="5">
-        <f>ROUNDDOWN(E60,0)</f>
+      <c r="G64" s="5">
+        <f>ROUNDDOWN(F64,0)</f>
         <v>62</v>
       </c>
-      <c r="G60">
-        <f t="shared" ref="G60:G62" si="0">$B$57-F60*C60</f>
+      <c r="H64">
+        <f t="shared" ref="H64:H66" si="0">$B$61-G64*D64</f>
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
         <v>2</v>
       </c>
-      <c r="B61">
-        <f t="shared" ref="B61:B64" si="1">A61*60</f>
+      <c r="C65">
+        <f t="shared" ref="C65:C68" si="1">B65*60</f>
         <v>120</v>
       </c>
-      <c r="C61">
+      <c r="D65">
         <v>7</v>
       </c>
-      <c r="D61">
-        <f t="shared" ref="D61:D64" si="2">2^C61</f>
+      <c r="E65">
+        <f t="shared" ref="E65:E68" si="2">2^D65</f>
         <v>128</v>
       </c>
-      <c r="E61" s="3">
-        <f>$B$57/C61</f>
+      <c r="F65" s="3">
+        <f>$B$61/D65</f>
         <v>53.714285714285715</v>
       </c>
-      <c r="F61" s="5">
-        <f t="shared" ref="F61:F64" si="3">ROUNDDOWN(E61,0)</f>
+      <c r="G65" s="5">
+        <f t="shared" ref="G65:G68" si="3">ROUNDDOWN(F65,0)</f>
         <v>53</v>
       </c>
-      <c r="G61">
+      <c r="H65">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66">
         <v>4</v>
       </c>
-      <c r="B62">
+      <c r="C66">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="C62">
+      <c r="D66">
         <v>8</v>
       </c>
-      <c r="D62">
+      <c r="E66">
         <f t="shared" si="2"/>
         <v>256</v>
       </c>
-      <c r="E62" s="3">
-        <f>$B$57/C62</f>
+      <c r="F66" s="3">
+        <f>$B$61/D66</f>
         <v>47</v>
       </c>
-      <c r="F62" s="5">
+      <c r="G66" s="5">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="G62">
+      <c r="H66">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>3</v>
+      </c>
+      <c r="B67">
         <v>8</v>
       </c>
-      <c r="B63">
+      <c r="C67">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="C63">
+      <c r="D67">
         <v>9</v>
       </c>
-      <c r="D63">
+      <c r="E67">
         <f t="shared" si="2"/>
         <v>512</v>
       </c>
-      <c r="E63" s="3">
-        <f>$B$57/C63</f>
+      <c r="F67" s="3">
+        <f>$B$61/D67</f>
         <v>41.777777777777779</v>
       </c>
-      <c r="F63" s="5">
+      <c r="G67" s="5">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="G63">
-        <f>$B$57-F63*C63</f>
+      <c r="H67">
+        <f>$B$61-G67*D67</f>
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>4</v>
+      </c>
+      <c r="B68">
         <v>17</v>
       </c>
-      <c r="B64">
+      <c r="C68">
         <f t="shared" si="1"/>
         <v>1020</v>
       </c>
-      <c r="C64">
+      <c r="D68">
         <v>10</v>
       </c>
-      <c r="D64">
+      <c r="E68">
         <f t="shared" si="2"/>
         <v>1024</v>
       </c>
-      <c r="E64" s="3">
-        <f>$B$57/C64</f>
+      <c r="F68" s="3">
+        <f>$B$61/D68</f>
         <v>37.6</v>
       </c>
-      <c r="F64" s="5">
+      <c r="G68" s="5">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="G64">
-        <f>$B$57-F64*C64</f>
+      <c r="H68">
+        <f>$B$61-G68*D68</f>
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E66" s="3"/>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E70" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2634,7 +2603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8852597E-F5BB-40E1-97DB-5D341DB313BD}">
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -2644,46 +2613,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="25" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="25" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="25" t="s">
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="27"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="19"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -2784,52 +2753,52 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="16" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="16" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="17"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="16" t="s">
+      <c r="O3" s="24"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="17"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="28" t="s">
+      <c r="R3" s="24"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="28" t="s">
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
-      <c r="AB3" s="29"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="28" t="s">
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="AE3" s="29"/>
-      <c r="AF3" s="30"/>
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="22"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
@@ -2974,44 +2943,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="11">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="K3" s="15" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="K3" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15" t="s">
+      <c r="L3" s="26"/>
+      <c r="M3" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="12">
         <v>0.01</v>
       </c>
@@ -3030,8 +2999,8 @@
       <c r="I4" s="12">
         <v>10</v>
       </c>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
       <c r="M4" s="12">
         <v>0.01</v>
       </c>
@@ -3052,7 +3021,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="27" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="12">
@@ -3082,7 +3051,7 @@
         <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="27" t="s">
         <v>50</v>
       </c>
       <c r="L5" s="12">
@@ -3114,7 +3083,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="12">
         <v>0.02</v>
       </c>
@@ -3142,7 +3111,7 @@
         <f t="shared" si="2"/>
         <v>2E-3</v>
       </c>
-      <c r="K6" s="23"/>
+      <c r="K6" s="27"/>
       <c r="L6" s="12">
         <v>0.02</v>
       </c>
@@ -3172,7 +3141,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="12">
         <v>0.03</v>
       </c>
@@ -3200,7 +3169,7 @@
         <f t="shared" si="2"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K7" s="23"/>
+      <c r="K7" s="27"/>
       <c r="L7" s="12">
         <v>0.03</v>
       </c>
@@ -3230,7 +3199,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="12">
         <v>0.05</v>
       </c>
@@ -3258,7 +3227,7 @@
         <f t="shared" si="2"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K8" s="23"/>
+      <c r="K8" s="27"/>
       <c r="L8" s="12">
         <v>0.05</v>
       </c>
@@ -3288,7 +3257,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="12">
         <v>0.1</v>
       </c>
@@ -3316,7 +3285,7 @@
         <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
-      <c r="K9" s="23"/>
+      <c r="K9" s="27"/>
       <c r="L9" s="12">
         <v>0.1</v>
       </c>
@@ -3346,7 +3315,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="12">
         <v>0.2</v>
       </c>
@@ -3374,7 +3343,7 @@
         <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
-      <c r="K10" s="23"/>
+      <c r="K10" s="27"/>
       <c r="L10" s="12">
         <v>0.2</v>
       </c>
@@ -3404,7 +3373,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="12">
         <v>0.3</v>
       </c>
@@ -3420,7 +3389,7 @@
         <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="15">
         <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
@@ -3432,7 +3401,7 @@
         <f t="shared" si="2"/>
         <v>0.03</v>
       </c>
-      <c r="K11" s="23"/>
+      <c r="K11" s="27"/>
       <c r="L11" s="12">
         <v>0.3</v>
       </c>
@@ -3448,7 +3417,7 @@
         <f t="shared" si="5"/>
         <v>0.18</v>
       </c>
-      <c r="P11" s="24">
+      <c r="P11" s="15">
         <f t="shared" si="6"/>
         <v>0.09</v>
       </c>
@@ -3462,7 +3431,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="23"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="12">
         <v>0.5</v>
       </c>
@@ -3490,7 +3459,7 @@
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
-      <c r="K12" s="23"/>
+      <c r="K12" s="27"/>
       <c r="L12" s="12">
         <v>0.5</v>
       </c>
@@ -3520,7 +3489,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="23"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="12">
         <v>1</v>
       </c>
@@ -3548,7 +3517,7 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="K13" s="23"/>
+      <c r="K13" s="27"/>
       <c r="L13" s="12">
         <v>1</v>
       </c>
@@ -3579,13 +3548,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="K3:L4"/>
     <mergeCell ref="M3:R3"/>
     <mergeCell ref="K5:K13"/>
     <mergeCell ref="B5:B13"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="B3:C4"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="K3:L4"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:I13">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
@@ -3728,24 +3697,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
@@ -3804,28 +3773,28 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="16" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="16" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="17"/>
-      <c r="P3" s="18"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="25"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -3881,21 +3850,21 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="14" t="s">
+      <c r="R6" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="14"/>
+      <c r="S6" s="28"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -3933,10 +3902,10 @@
       <c r="Q7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R7" s="21" t="s">
+      <c r="R7" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="S7" s="21"/>
+      <c r="S7" s="30"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
@@ -3947,18 +3916,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14" t="s">
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
@@ -3972,18 +3941,18 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="14">
+      <c r="I9" s="28">
         <v>17</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14">
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28">
         <v>4</v>
       </c>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
@@ -4002,11 +3971,11 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="14" t="s">
+      <c r="N10" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -4025,18 +3994,24 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="20">
+      <c r="N11" s="29">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -4044,12 +4019,6 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rtc behavior bug fixed
</commit_message>
<xml_diff>
--- a/hardware/DataPackage.xlsx
+++ b/hardware/DataPackage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\Repos\lora\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54C1F69-F480-4D13-A3FC-242BF3636A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39E0AD8-EBBB-4DFE-8A8D-957E38BFC4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="2748" windowWidth="21252" windowHeight="12636" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="19308" yWindow="156" windowWidth="25644" windowHeight="15960" activeTab="1" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
   <si>
     <t>minutes of day</t>
   </si>
@@ -139,30 +139,6 @@
     <t>Messages</t>
   </si>
   <si>
-    <t>0 = no error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 = </t>
-  </si>
-  <si>
     <t>min. Temp [°C]</t>
   </si>
   <si>
@@ -220,13 +196,52 @@
     <t>4 byte</t>
   </si>
   <si>
-    <t>Spare</t>
-  </si>
-  <si>
     <t>Intervall index</t>
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>0A</t>
+  </si>
+  <si>
+    <t>Intervall id</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Battery Level [%]</t>
+  </si>
+  <si>
+    <t>Humidity [%]</t>
+  </si>
+  <si>
+    <t>Temperatur [°C]</t>
+  </si>
+  <si>
+    <t>Hour of the day</t>
+  </si>
+  <si>
+    <t>Intervall [h]</t>
+  </si>
+  <si>
+    <t>no error</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>88</t>
   </si>
 </sst>
 </file>
@@ -429,7 +444,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -466,6 +481,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -496,13 +517,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -511,11 +535,17 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1966,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FF0E6-8FE4-49E3-812F-B76B934E1ACD}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1976,7 +2006,7 @@
     <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1984,7 +2014,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1993,12 +2023,12 @@
         <v>408</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2006,7 +2036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2014,7 +2044,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2023,18 +2053,21 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -2042,11 +2075,11 @@
         <f>2^B11</f>
         <v>8</v>
       </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2054,26 +2087,26 @@
         <f>B8-B11</f>
         <v>397</v>
       </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" t="s">
         <v>38</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2083,8 +2116,8 @@
       <c r="B17">
         <v>5</v>
       </c>
-      <c r="D17" t="s">
-        <v>39</v>
+      <c r="D17">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2095,8 +2128,8 @@
         <f>100/(2^B17-1)</f>
         <v>3.225806451612903</v>
       </c>
-      <c r="D18" t="s">
-        <v>40</v>
+      <c r="D18">
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2110,7 +2143,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2123,7 +2156,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B24">
         <v>-20</v>
@@ -2131,7 +2164,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B25">
         <v>50</v>
@@ -2139,7 +2172,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B26">
         <f>B25-B24</f>
@@ -2148,7 +2181,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2">
         <f>B26/(2^B23-1)</f>
@@ -2167,7 +2200,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2198,7 +2231,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2219,14 +2252,14 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
@@ -2277,14 +2310,14 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
@@ -2296,7 +2329,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="1"/>
@@ -2320,7 +2353,7 @@
       <c r="A55" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="32">
+      <c r="B55" s="17">
         <f>B39-B54</f>
         <v>381</v>
       </c>
@@ -2387,7 +2420,7 @@
         <v>376</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D61" s="1">
         <f>B61/8</f>
@@ -2404,7 +2437,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
@@ -2601,10 +2634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8852597E-F5BB-40E1-97DB-5D341DB313BD}">
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AF20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH27" sqref="AH27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2613,46 +2646,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="19"/>
+      <c r="A1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="21"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -2753,52 +2786,52 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="23" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="23" t="s">
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="26"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="26"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="24"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" s="24"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="22"/>
-      <c r="Y3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="22"/>
-      <c r="AD3" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE3" s="21"/>
-      <c r="AF3" s="22"/>
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="24"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
@@ -2822,88 +2855,836 @@
       <c r="S4" s="11"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
+      <c r="A5" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
+      <c r="Z5" s="31"/>
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
+      <c r="AC5" s="31"/>
+      <c r="AD5" s="31"/>
+      <c r="AE5" s="31"/>
+      <c r="AF5" s="31"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="A6" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35">
+        <v>38</v>
+      </c>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="35">
+        <v>73</v>
+      </c>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35"/>
+      <c r="V6" s="35"/>
+      <c r="W6" s="35"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="35">
+        <v>88</v>
+      </c>
+      <c r="Z6" s="35"/>
+      <c r="AA6" s="35"/>
+      <c r="AB6" s="35"/>
+      <c r="AC6" s="35"/>
+      <c r="AD6" s="35"/>
+      <c r="AE6" s="35"/>
+      <c r="AF6" s="35"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="A7" s="16">
+        <v>0</v>
+      </c>
+      <c r="B7" s="16">
+        <v>0</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16">
+        <v>1</v>
+      </c>
+      <c r="H7" s="16">
+        <v>0</v>
+      </c>
+      <c r="I7" s="16">
+        <v>0</v>
+      </c>
+      <c r="J7" s="16">
+        <v>0</v>
+      </c>
+      <c r="K7" s="16">
+        <v>1</v>
+      </c>
+      <c r="L7" s="16">
+        <v>1</v>
+      </c>
+      <c r="M7" s="16">
+        <v>1</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0</v>
+      </c>
+      <c r="P7" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="16">
+        <v>0</v>
+      </c>
+      <c r="R7" s="16">
+        <v>1</v>
+      </c>
+      <c r="S7" s="16">
+        <v>1</v>
+      </c>
+      <c r="T7" s="16">
+        <v>1</v>
+      </c>
+      <c r="U7" s="16">
+        <v>0</v>
+      </c>
+      <c r="V7" s="16">
+        <v>0</v>
+      </c>
+      <c r="W7" s="16">
+        <v>1</v>
+      </c>
+      <c r="X7" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="16">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="16">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="16">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="A8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z8" s="28"/>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="28"/>
+      <c r="AD8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE8" s="28"/>
+      <c r="AF8" s="28"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="A9" s="28">
+        <v>10</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28">
+        <v>7</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28">
+        <v>0</v>
+      </c>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28">
+        <v>3</v>
+      </c>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28">
+        <v>19</v>
+      </c>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28">
+        <v>17</v>
+      </c>
+      <c r="Z9" s="28"/>
+      <c r="AA9" s="28"/>
+      <c r="AB9" s="28"/>
+      <c r="AC9" s="28"/>
+      <c r="AD9" s="28">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="28"/>
+      <c r="AF9" s="28"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="A10" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="28"/>
+      <c r="AD10" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE10" s="28"/>
+      <c r="AF10" s="28"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="A11" s="28">
+        <f>A9</f>
+        <v>10</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="32">
+        <f>100/(2^5-1)*I9</f>
+        <v>22.58064516129032</v>
+      </c>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="36" t="str">
+        <f>LOOKUP(N9,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$18)</f>
+        <v>no error</v>
+      </c>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="37">
+        <f>100/(2^3-1)*Q9</f>
+        <v>42.857142857142861</v>
+      </c>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37">
+        <f>'Data package'!$B$27*T9+'Data package'!$B$24</f>
+        <v>22.903225806451616</v>
+      </c>
+      <c r="U11" s="36"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="36"/>
+      <c r="Y11" s="36">
+        <f>Y9</f>
+        <v>17</v>
+      </c>
+      <c r="Z11" s="36"/>
+      <c r="AA11" s="36"/>
+      <c r="AB11" s="36"/>
+      <c r="AC11" s="36"/>
+      <c r="AD11" s="36">
+        <f>LOOKUP(AD9,'Data package'!$A$64:$A$68,'Data package'!$B$64:$B$68)</f>
+        <v>1</v>
+      </c>
+      <c r="AE11" s="36"/>
+      <c r="AF11" s="36"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A14" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="31"/>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="31"/>
+      <c r="AC14" s="31"/>
+      <c r="AD14" s="31"/>
+      <c r="AE14" s="31"/>
+      <c r="AF14" s="31"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="35"/>
+      <c r="U15" s="35"/>
+      <c r="V15" s="35"/>
+      <c r="W15" s="35"/>
+      <c r="X15" s="35"/>
+      <c r="Y15" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z15" s="35"/>
+      <c r="AA15" s="35"/>
+      <c r="AB15" s="35"/>
+      <c r="AC15" s="35"/>
+      <c r="AD15" s="35"/>
+      <c r="AE15" s="35"/>
+      <c r="AF15" s="35"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>0</v>
+      </c>
+      <c r="B16" s="16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="16">
+        <v>1</v>
+      </c>
+      <c r="I16" s="16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="16">
+        <v>0</v>
+      </c>
+      <c r="M16" s="16">
+        <v>0</v>
+      </c>
+      <c r="N16" s="16">
+        <v>0</v>
+      </c>
+      <c r="O16" s="16">
+        <v>0</v>
+      </c>
+      <c r="P16" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="16">
+        <v>0</v>
+      </c>
+      <c r="R16" s="16">
+        <v>1</v>
+      </c>
+      <c r="S16" s="16">
+        <v>1</v>
+      </c>
+      <c r="T16" s="16">
+        <v>1</v>
+      </c>
+      <c r="U16" s="16">
+        <v>0</v>
+      </c>
+      <c r="V16" s="16">
+        <v>0</v>
+      </c>
+      <c r="W16" s="16">
+        <v>1</v>
+      </c>
+      <c r="X16" s="16">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="16">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="16">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="16">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A17" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="U17" s="28"/>
+      <c r="V17" s="28"/>
+      <c r="W17" s="28"/>
+      <c r="X17" s="28"/>
+      <c r="Y17" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z17" s="28"/>
+      <c r="AA17" s="28"/>
+      <c r="AB17" s="28"/>
+      <c r="AC17" s="28"/>
+      <c r="AD17" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE17" s="28"/>
+      <c r="AF17" s="28"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A18" s="28">
+        <v>5</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28">
+        <v>8</v>
+      </c>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28">
+        <v>0</v>
+      </c>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28">
+        <v>3</v>
+      </c>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28">
+        <v>19</v>
+      </c>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="28"/>
+      <c r="X18" s="28"/>
+      <c r="Y18" s="28">
+        <v>17</v>
+      </c>
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="28"/>
+      <c r="AD18" s="28">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="28"/>
+      <c r="AF18" s="28"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A19" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="28"/>
+      <c r="AB19" s="28"/>
+      <c r="AC19" s="28"/>
+      <c r="AD19" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="28"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A20" s="28">
+        <f>A18</f>
+        <v>5</v>
+      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="32">
+        <f>100/(2^5-1)*I18</f>
+        <v>25.806451612903224</v>
+      </c>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="36" t="str">
+        <f>LOOKUP(N18,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$18)</f>
+        <v>no error</v>
+      </c>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="37">
+        <f>100/(2^3-1)*Q18</f>
+        <v>42.857142857142861</v>
+      </c>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="37">
+        <f>'Data package'!$B$27*T18+'Data package'!$B$24</f>
+        <v>22.903225806451616</v>
+      </c>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36"/>
+      <c r="Y20" s="36">
+        <f>Y18</f>
+        <v>17</v>
+      </c>
+      <c r="Z20" s="36"/>
+      <c r="AA20" s="36"/>
+      <c r="AB20" s="36"/>
+      <c r="AC20" s="36"/>
+      <c r="AD20" s="36">
+        <f>LOOKUP(AD18,'Data package'!$A$64:$A$68,'Data package'!$B$64:$B$68)</f>
+        <v>1</v>
+      </c>
+      <c r="AE20" s="36"/>
+      <c r="AF20" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="77">
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="Y20:AC20"/>
+    <mergeCell ref="AD20:AF20"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="Q15:X15"/>
+    <mergeCell ref="Y15:AF15"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="T9:X9"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="Y6:AF6"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="A5:AF5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="I6:P6"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="I9:M9"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="I1:P1"/>
     <mergeCell ref="Q1:X1"/>
@@ -2944,7 +3725,7 @@
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B1" s="28" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -2953,34 +3734,34 @@
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="K3" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
+      <c r="B3" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="K3" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="12">
         <v>0.01</v>
       </c>
@@ -2999,8 +3780,8 @@
       <c r="I4" s="12">
         <v>10</v>
       </c>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
       <c r="M4" s="12">
         <v>0.01</v>
       </c>
@@ -3021,8 +3802,8 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="27" t="s">
-        <v>50</v>
+      <c r="B5" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="C5" s="12">
         <v>0.01</v>
@@ -3051,8 +3832,8 @@
         <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="K5" s="27" t="s">
-        <v>50</v>
+      <c r="K5" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="L5" s="12">
         <v>0.01</v>
@@ -3083,7 +3864,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="27"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="12">
         <v>0.02</v>
       </c>
@@ -3111,7 +3892,7 @@
         <f t="shared" si="2"/>
         <v>2E-3</v>
       </c>
-      <c r="K6" s="27"/>
+      <c r="K6" s="30"/>
       <c r="L6" s="12">
         <v>0.02</v>
       </c>
@@ -3141,7 +3922,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="27"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="12">
         <v>0.03</v>
       </c>
@@ -3169,7 +3950,7 @@
         <f t="shared" si="2"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K7" s="27"/>
+      <c r="K7" s="30"/>
       <c r="L7" s="12">
         <v>0.03</v>
       </c>
@@ -3199,7 +3980,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="27"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="12">
         <v>0.05</v>
       </c>
@@ -3227,7 +4008,7 @@
         <f t="shared" si="2"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K8" s="27"/>
+      <c r="K8" s="30"/>
       <c r="L8" s="12">
         <v>0.05</v>
       </c>
@@ -3257,7 +4038,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="27"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="12">
         <v>0.1</v>
       </c>
@@ -3285,7 +4066,7 @@
         <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
-      <c r="K9" s="27"/>
+      <c r="K9" s="30"/>
       <c r="L9" s="12">
         <v>0.1</v>
       </c>
@@ -3315,7 +4096,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="27"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="12">
         <v>0.2</v>
       </c>
@@ -3343,7 +4124,7 @@
         <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
-      <c r="K10" s="27"/>
+      <c r="K10" s="30"/>
       <c r="L10" s="12">
         <v>0.2</v>
       </c>
@@ -3373,7 +4154,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="27"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="12">
         <v>0.3</v>
       </c>
@@ -3401,7 +4182,7 @@
         <f t="shared" si="2"/>
         <v>0.03</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="K11" s="30"/>
       <c r="L11" s="12">
         <v>0.3</v>
       </c>
@@ -3431,7 +4212,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="27"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="12">
         <v>0.5</v>
       </c>
@@ -3459,7 +4240,7 @@
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
-      <c r="K12" s="27"/>
+      <c r="K12" s="30"/>
       <c r="L12" s="12">
         <v>0.5</v>
       </c>
@@ -3489,7 +4270,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="27"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="12">
         <v>1</v>
       </c>
@@ -3517,7 +4298,7 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="K13" s="27"/>
+      <c r="K13" s="30"/>
       <c r="L13" s="12">
         <v>1</v>
       </c>
@@ -3688,7 +4469,7 @@
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:M3"/>
+      <selection activeCell="I6" sqref="I6:S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3697,24 +4478,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
@@ -3773,28 +4554,28 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="23" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="23" t="s">
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="24"/>
-      <c r="P3" s="25"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="27"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -3902,10 +4683,10 @@
       <c r="Q7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R7" s="30" t="s">
+      <c r="R7" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="S7" s="30"/>
+      <c r="S7" s="33"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
@@ -3994,24 +4775,18 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="29">
+      <c r="N11" s="32">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -4019,6 +4794,12 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Data package time array bug fixed and example decoding added
</commit_message>
<xml_diff>
--- a/hardware/DataPackage.xlsx
+++ b/hardware/DataPackage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\Repos\lora\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39E0AD8-EBBB-4DFE-8A8D-957E38BFC4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F0268F-2BFF-4595-83FC-F7B8E56D10B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19308" yWindow="156" windowWidth="25644" windowHeight="15960" activeTab="1" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="15636" yWindow="156" windowWidth="25644" windowHeight="15960" activeTab="1" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="84">
   <si>
     <t>minutes of day</t>
   </si>
@@ -242,6 +242,54 @@
   </si>
   <si>
     <t>88</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>9A</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Inv</t>
+  </si>
+  <si>
+    <t>1. count</t>
+  </si>
+  <si>
+    <t>2. count</t>
+  </si>
+  <si>
+    <t>3. count</t>
+  </si>
+  <si>
+    <t>4. count</t>
+  </si>
+  <si>
+    <t>5. count</t>
+  </si>
+  <si>
+    <t>6. count</t>
+  </si>
+  <si>
+    <t>7. count</t>
+  </si>
+  <si>
+    <t>8. count</t>
+  </si>
+  <si>
+    <t>9. count</t>
+  </si>
+  <si>
+    <t>10. count</t>
+  </si>
+  <si>
+    <t>min. of hour</t>
   </si>
 </sst>
 </file>
@@ -444,7 +492,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -487,8 +535,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -517,34 +589,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1996,7 +2050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FF0E6-8FE4-49E3-812F-B76B934E1ACD}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2252,14 +2306,14 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
@@ -2310,14 +2364,14 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
@@ -2634,58 +2688,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8852597E-F5BB-40E1-97DB-5D341DB313BD}">
-  <dimension ref="A1:AF20"/>
+  <dimension ref="A1:CR32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH27" sqref="AH27"/>
+      <selection activeCell="AK17" sqref="AK17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="32" width="4.21875" customWidth="1"/>
+    <col min="33" max="150" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="19" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="19" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="19" t="s">
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="21"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="29"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -2786,52 +2841,52 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="25" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="25" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="26"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="25" t="s">
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="26"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="22" t="s">
+      <c r="R3" s="34"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="22" t="s">
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="22" t="s">
+      <c r="Z3" s="31"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="32"/>
+      <c r="AD3" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="24"/>
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="32"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
@@ -2855,82 +2910,82 @@
       <c r="S4" s="11"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31"/>
-      <c r="Z5" s="31"/>
-      <c r="AA5" s="31"/>
-      <c r="AB5" s="31"/>
-      <c r="AC5" s="31"/>
-      <c r="AD5" s="31"/>
-      <c r="AE5" s="31"/>
-      <c r="AF5" s="31"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="26"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35">
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25">
         <v>38</v>
       </c>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35">
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25">
         <v>73</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35">
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25">
         <v>88</v>
       </c>
-      <c r="Z6" s="35"/>
-      <c r="AA6" s="35"/>
-      <c r="AB6" s="35"/>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="35"/>
-      <c r="AE6" s="35"/>
-      <c r="AF6" s="35"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="25"/>
+      <c r="AD6" s="25"/>
+      <c r="AE6" s="25"/>
+      <c r="AF6" s="25"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
@@ -3031,203 +3086,203 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28" t="s">
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28" t="s">
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="28" t="s">
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="28"/>
-      <c r="V8" s="28"/>
-      <c r="W8" s="28"/>
-      <c r="X8" s="28"/>
-      <c r="Y8" s="28" t="s">
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="28"/>
-      <c r="AA8" s="28"/>
-      <c r="AB8" s="28"/>
-      <c r="AC8" s="28"/>
-      <c r="AD8" s="28" t="s">
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="AE8" s="28"/>
-      <c r="AF8" s="28"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="21"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="28">
+      <c r="A9" s="21">
         <v>10</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28">
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21">
         <v>7</v>
       </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28">
-        <v>0</v>
-      </c>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28">
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21">
+        <v>0</v>
+      </c>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21">
         <v>3</v>
       </c>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28">
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21">
         <v>19</v>
       </c>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28">
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="21">
         <v>17</v>
       </c>
-      <c r="Z9" s="28"/>
-      <c r="AA9" s="28"/>
-      <c r="AB9" s="28"/>
-      <c r="AC9" s="28"/>
-      <c r="AD9" s="28">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="28"/>
-      <c r="AF9" s="28"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="21"/>
+      <c r="AB9" s="21"/>
+      <c r="AC9" s="21"/>
+      <c r="AD9" s="21">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="21"/>
+      <c r="AF9" s="21"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28" t="s">
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28" t="s">
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
-      <c r="T10" s="28" t="s">
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="U10" s="28"/>
-      <c r="V10" s="28"/>
-      <c r="W10" s="28"/>
-      <c r="X10" s="28"/>
-      <c r="Y10" s="28" t="s">
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="Z10" s="28"/>
-      <c r="AA10" s="28"/>
-      <c r="AB10" s="28"/>
-      <c r="AC10" s="28"/>
-      <c r="AD10" s="28" t="s">
+      <c r="Z10" s="21"/>
+      <c r="AA10" s="21"/>
+      <c r="AB10" s="21"/>
+      <c r="AC10" s="21"/>
+      <c r="AD10" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="AE10" s="28"/>
-      <c r="AF10" s="28"/>
+      <c r="AE10" s="21"/>
+      <c r="AF10" s="21"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="28">
+      <c r="A11" s="21">
         <f>A9</f>
         <v>10</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="32">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22">
         <f>100/(2^5-1)*I9</f>
         <v>22.58064516129032</v>
       </c>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="36" t="str">
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="23" t="str">
         <f>LOOKUP(N9,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$18)</f>
         <v>no error</v>
       </c>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="37">
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="24">
         <f>100/(2^3-1)*Q9</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R11" s="37"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="37">
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24">
         <f>'Data package'!$B$27*T9+'Data package'!$B$24</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U11" s="36"/>
-      <c r="V11" s="36"/>
-      <c r="W11" s="36"/>
-      <c r="X11" s="36"/>
-      <c r="Y11" s="36">
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="23"/>
+      <c r="Y11" s="23">
         <f>Y9</f>
         <v>17</v>
       </c>
-      <c r="Z11" s="36"/>
-      <c r="AA11" s="36"/>
-      <c r="AB11" s="36"/>
-      <c r="AC11" s="36"/>
-      <c r="AD11" s="36">
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="23"/>
+      <c r="AB11" s="23"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="23">
         <f>LOOKUP(AD9,'Data package'!$A$64:$A$68,'Data package'!$B$64:$B$68)</f>
         <v>1</v>
       </c>
-      <c r="AE11" s="36"/>
-      <c r="AF11" s="36"/>
+      <c r="AE11" s="23"/>
+      <c r="AF11" s="23"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
@@ -3235,90 +3290,90 @@
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="31"/>
-      <c r="Y14" s="31"/>
-      <c r="Z14" s="31"/>
-      <c r="AA14" s="31"/>
-      <c r="AB14" s="31"/>
-      <c r="AC14" s="31"/>
-      <c r="AD14" s="31"/>
-      <c r="AE14" s="31"/>
-      <c r="AF14" s="31"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="26"/>
+      <c r="AB14" s="26"/>
+      <c r="AC14" s="26"/>
+      <c r="AD14" s="26"/>
+      <c r="AE14" s="26"/>
+      <c r="AF14" s="26"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35" t="s">
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
-      <c r="X15" s="35"/>
-      <c r="Y15" s="35" t="s">
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="25"/>
+      <c r="Y15" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="Z15" s="35"/>
-      <c r="AA15" s="35"/>
-      <c r="AB15" s="35"/>
-      <c r="AC15" s="35"/>
-      <c r="AD15" s="35"/>
-      <c r="AE15" s="35"/>
-      <c r="AF15" s="35"/>
+      <c r="Z15" s="25"/>
+      <c r="AA15" s="25"/>
+      <c r="AB15" s="25"/>
+      <c r="AC15" s="25"/>
+      <c r="AD15" s="25"/>
+      <c r="AE15" s="25"/>
+      <c r="AF15" s="25"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
@@ -3418,207 +3473,1908 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+    <row r="17" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28" t="s">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28" t="s">
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28" t="s">
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="28"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="28" t="s">
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="U17" s="28"/>
-      <c r="V17" s="28"/>
-      <c r="W17" s="28"/>
-      <c r="X17" s="28"/>
-      <c r="Y17" s="28" t="s">
+      <c r="U17" s="21"/>
+      <c r="V17" s="21"/>
+      <c r="W17" s="21"/>
+      <c r="X17" s="21"/>
+      <c r="Y17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="28"/>
-      <c r="AA17" s="28"/>
-      <c r="AB17" s="28"/>
-      <c r="AC17" s="28"/>
-      <c r="AD17" s="28" t="s">
+      <c r="Z17" s="21"/>
+      <c r="AA17" s="21"/>
+      <c r="AB17" s="21"/>
+      <c r="AC17" s="21"/>
+      <c r="AD17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="28"/>
-      <c r="AF17" s="28"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A18" s="28">
+      <c r="AE17" s="21"/>
+      <c r="AF17" s="21"/>
+    </row>
+    <row r="18" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A18" s="21">
         <v>5</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21">
         <v>8</v>
       </c>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28">
-        <v>0</v>
-      </c>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28">
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21">
+        <v>0</v>
+      </c>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21">
         <v>3</v>
       </c>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="28">
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21">
         <v>19</v>
       </c>
-      <c r="U18" s="28"/>
-      <c r="V18" s="28"/>
-      <c r="W18" s="28"/>
-      <c r="X18" s="28"/>
-      <c r="Y18" s="28">
+      <c r="U18" s="21"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="21">
         <v>17</v>
       </c>
-      <c r="Z18" s="28"/>
-      <c r="AA18" s="28"/>
-      <c r="AB18" s="28"/>
-      <c r="AC18" s="28"/>
-      <c r="AD18" s="28">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="28"/>
-      <c r="AF18" s="28"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="21"/>
+      <c r="AB18" s="21"/>
+      <c r="AC18" s="21"/>
+      <c r="AD18" s="21">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="21"/>
+      <c r="AF18" s="21"/>
+    </row>
+    <row r="19" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28" t="s">
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="O19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="28" t="s">
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="R19" s="28"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28" t="s">
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="U19" s="28"/>
-      <c r="V19" s="28"/>
-      <c r="W19" s="28"/>
-      <c r="X19" s="28"/>
-      <c r="Y19" s="28" t="s">
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="28"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="28"/>
-      <c r="AD19" s="28" t="s">
+      <c r="Z19" s="21"/>
+      <c r="AA19" s="21"/>
+      <c r="AB19" s="21"/>
+      <c r="AC19" s="21"/>
+      <c r="AD19" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="AE19" s="28"/>
-      <c r="AF19" s="28"/>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A20" s="28">
+      <c r="AE19" s="21"/>
+      <c r="AF19" s="21"/>
+    </row>
+    <row r="20" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A20" s="21">
         <f>A18</f>
         <v>5</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="32">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22">
         <f>100/(2^5-1)*I18</f>
         <v>25.806451612903224</v>
       </c>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="36" t="str">
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="23" t="str">
         <f>LOOKUP(N18,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$18)</f>
         <v>no error</v>
       </c>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="37">
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="24">
         <f>100/(2^3-1)*Q18</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="37">
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24">
         <f>'Data package'!$B$27*T18+'Data package'!$B$24</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="36">
+      <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="23">
         <f>Y18</f>
         <v>17</v>
       </c>
-      <c r="Z20" s="36"/>
-      <c r="AA20" s="36"/>
-      <c r="AB20" s="36"/>
-      <c r="AC20" s="36"/>
-      <c r="AD20" s="36">
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="23"/>
+      <c r="AC20" s="23"/>
+      <c r="AD20" s="23">
         <f>LOOKUP(AD18,'Data package'!$A$64:$A$68,'Data package'!$B$64:$B$68)</f>
         <v>1</v>
       </c>
-      <c r="AE20" s="36"/>
-      <c r="AF20" s="36"/>
+      <c r="AE20" s="23"/>
+      <c r="AF20" s="23"/>
+    </row>
+    <row r="23" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A23" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26"/>
+      <c r="V23" s="26"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="26"/>
+      <c r="Z23" s="26"/>
+      <c r="AA23" s="26"/>
+      <c r="AB23" s="26"/>
+      <c r="AC23" s="26"/>
+      <c r="AD23" s="26"/>
+      <c r="AE23" s="26"/>
+      <c r="AF23" s="26"/>
+    </row>
+    <row r="24" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A24" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="25"/>
+      <c r="X24" s="25"/>
+      <c r="Y24" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z24" s="25"/>
+      <c r="AA24" s="25"/>
+      <c r="AB24" s="25"/>
+      <c r="AC24" s="25"/>
+      <c r="AD24" s="25"/>
+      <c r="AE24" s="25"/>
+      <c r="AF24" s="25"/>
+      <c r="AG24" s="39">
+        <v>59</v>
+      </c>
+      <c r="AH24" s="39"/>
+      <c r="AI24" s="39"/>
+      <c r="AJ24" s="39"/>
+      <c r="AK24" s="39"/>
+      <c r="AL24" s="39"/>
+      <c r="AM24" s="39"/>
+      <c r="AN24" s="39"/>
+      <c r="AO24" s="39">
+        <v>96</v>
+      </c>
+      <c r="AP24" s="39"/>
+      <c r="AQ24" s="39"/>
+      <c r="AR24" s="39"/>
+      <c r="AS24" s="39"/>
+      <c r="AT24" s="39"/>
+      <c r="AU24" s="39"/>
+      <c r="AV24" s="39"/>
+      <c r="AW24" s="39">
+        <v>65</v>
+      </c>
+      <c r="AX24" s="39"/>
+      <c r="AY24" s="39"/>
+      <c r="AZ24" s="39"/>
+      <c r="BA24" s="39"/>
+      <c r="BB24" s="39"/>
+      <c r="BC24" s="39"/>
+      <c r="BD24" s="39"/>
+      <c r="BE24" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="BF24" s="39"/>
+      <c r="BG24" s="39"/>
+      <c r="BH24" s="39"/>
+      <c r="BI24" s="39"/>
+      <c r="BJ24" s="39"/>
+      <c r="BK24" s="39"/>
+      <c r="BL24" s="39"/>
+      <c r="BM24" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="BN24" s="39"/>
+      <c r="BO24" s="39"/>
+      <c r="BP24" s="39"/>
+      <c r="BQ24" s="39"/>
+      <c r="BR24" s="39"/>
+      <c r="BS24" s="39"/>
+      <c r="BT24" s="39"/>
+      <c r="BU24" s="39">
+        <v>69</v>
+      </c>
+      <c r="BV24" s="39"/>
+      <c r="BW24" s="39"/>
+      <c r="BX24" s="39"/>
+      <c r="BY24" s="39"/>
+      <c r="BZ24" s="39"/>
+      <c r="CA24" s="39"/>
+      <c r="CB24" s="39"/>
+      <c r="CC24" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="CD24" s="39"/>
+      <c r="CE24" s="39"/>
+      <c r="CF24" s="39"/>
+      <c r="CG24" s="39"/>
+      <c r="CH24" s="39"/>
+      <c r="CI24" s="39"/>
+      <c r="CJ24" s="39"/>
+      <c r="CK24" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="CL24" s="39"/>
+      <c r="CM24" s="39"/>
+      <c r="CN24" s="39"/>
+      <c r="CO24" s="39"/>
+      <c r="CP24" s="39"/>
+      <c r="CQ24" s="39"/>
+      <c r="CR24" s="39"/>
+    </row>
+    <row r="25" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A25" s="18">
+        <v>0</v>
+      </c>
+      <c r="B25" s="18">
+        <v>0</v>
+      </c>
+      <c r="C25" s="18">
+        <v>0</v>
+      </c>
+      <c r="D25" s="18">
+        <v>0</v>
+      </c>
+      <c r="E25" s="18">
+        <v>1</v>
+      </c>
+      <c r="F25" s="18">
+        <v>0</v>
+      </c>
+      <c r="G25" s="18">
+        <v>1</v>
+      </c>
+      <c r="H25" s="18">
+        <v>0</v>
+      </c>
+      <c r="I25" s="18">
+        <v>0</v>
+      </c>
+      <c r="J25" s="18">
+        <v>1</v>
+      </c>
+      <c r="K25" s="18">
+        <v>0</v>
+      </c>
+      <c r="L25" s="18">
+        <v>0</v>
+      </c>
+      <c r="M25" s="18">
+        <v>0</v>
+      </c>
+      <c r="N25" s="18">
+        <v>0</v>
+      </c>
+      <c r="O25" s="18">
+        <v>0</v>
+      </c>
+      <c r="P25" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="18">
+        <v>0</v>
+      </c>
+      <c r="R25" s="18">
+        <v>1</v>
+      </c>
+      <c r="S25" s="18">
+        <v>1</v>
+      </c>
+      <c r="T25" s="18">
+        <v>1</v>
+      </c>
+      <c r="U25" s="18">
+        <v>0</v>
+      </c>
+      <c r="V25" s="18">
+        <v>0</v>
+      </c>
+      <c r="W25" s="18">
+        <v>1</v>
+      </c>
+      <c r="X25" s="18">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="18">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AI25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AK25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AL25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AN25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AO25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AP25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AQ25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AR25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AS25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AT25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AU25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AV25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AW25" s="18">
+        <v>0</v>
+      </c>
+      <c r="AX25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AY25" s="18">
+        <v>1</v>
+      </c>
+      <c r="AZ25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BA25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BB25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BC25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BD25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BE25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BF25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BG25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BH25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BI25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BJ25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BK25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BL25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BM25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BN25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BO25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BP25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BQ25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BR25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BS25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BT25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BU25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BV25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BW25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BX25" s="18">
+        <v>0</v>
+      </c>
+      <c r="BY25" s="18">
+        <v>1</v>
+      </c>
+      <c r="BZ25" s="18">
+        <v>0</v>
+      </c>
+      <c r="CA25" s="18">
+        <v>0</v>
+      </c>
+      <c r="CB25" s="18">
+        <v>1</v>
+      </c>
+      <c r="CC25" s="18">
+        <v>1</v>
+      </c>
+      <c r="CD25" s="18">
+        <v>0</v>
+      </c>
+      <c r="CE25" s="18">
+        <v>0</v>
+      </c>
+      <c r="CF25" s="18">
+        <v>1</v>
+      </c>
+      <c r="CG25" s="18">
+        <v>1</v>
+      </c>
+      <c r="CH25" s="18">
+        <v>0</v>
+      </c>
+      <c r="CI25" s="18">
+        <v>1</v>
+      </c>
+      <c r="CJ25" s="18">
+        <v>0</v>
+      </c>
+      <c r="CK25" s="18">
+        <v>0</v>
+      </c>
+      <c r="CL25" s="18">
+        <v>0</v>
+      </c>
+      <c r="CM25" s="18">
+        <v>0</v>
+      </c>
+      <c r="CN25" s="18">
+        <v>0</v>
+      </c>
+      <c r="CO25" s="18">
+        <v>0</v>
+      </c>
+      <c r="CP25" s="18">
+        <v>1</v>
+      </c>
+      <c r="CQ25" s="18">
+        <v>1</v>
+      </c>
+      <c r="CR25" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z26" s="21"/>
+      <c r="AA26" s="21"/>
+      <c r="AB26" s="21"/>
+      <c r="AC26" s="21"/>
+      <c r="AD26" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE26" s="21"/>
+      <c r="AF26" s="21"/>
+      <c r="AG26" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH26" s="23"/>
+      <c r="AI26" s="23"/>
+      <c r="AJ26" s="23"/>
+      <c r="AK26" s="23"/>
+      <c r="AL26" s="23"/>
+      <c r="AM26" s="23"/>
+      <c r="AN26" s="23"/>
+      <c r="AO26" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP26" s="23"/>
+      <c r="AQ26" s="23"/>
+      <c r="AR26" s="23"/>
+      <c r="AS26" s="23"/>
+      <c r="AT26" s="23"/>
+      <c r="AU26" s="23"/>
+      <c r="AV26" s="23"/>
+      <c r="AW26" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AX26" s="23"/>
+      <c r="AY26" s="23"/>
+      <c r="AZ26" s="23"/>
+      <c r="BA26" s="23"/>
+      <c r="BB26" s="23"/>
+      <c r="BC26" s="23"/>
+      <c r="BD26" s="23"/>
+      <c r="BE26" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="BF26" s="23"/>
+      <c r="BG26" s="23"/>
+      <c r="BH26" s="23"/>
+      <c r="BI26" s="23"/>
+      <c r="BJ26" s="23"/>
+      <c r="BK26" s="23"/>
+      <c r="BL26" s="23"/>
+      <c r="BM26" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="BN26" s="23"/>
+      <c r="BO26" s="23"/>
+      <c r="BP26" s="23"/>
+      <c r="BQ26" s="23"/>
+      <c r="BR26" s="23"/>
+      <c r="BS26" s="23"/>
+      <c r="BT26" s="23"/>
+      <c r="BU26" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV26" s="23"/>
+      <c r="BW26" s="23"/>
+      <c r="BX26" s="23"/>
+      <c r="BY26" s="23"/>
+      <c r="BZ26" s="23"/>
+      <c r="CA26" s="23"/>
+      <c r="CB26" s="23"/>
+      <c r="CC26" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="CD26" s="23"/>
+      <c r="CE26" s="23"/>
+      <c r="CF26" s="23"/>
+      <c r="CG26" s="23"/>
+      <c r="CH26" s="23"/>
+      <c r="CI26" s="23"/>
+      <c r="CJ26" s="23"/>
+      <c r="CK26" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="CL26" s="23"/>
+      <c r="CM26" s="23"/>
+      <c r="CN26" s="23"/>
+      <c r="CO26" s="23"/>
+      <c r="CP26" s="23"/>
+      <c r="CQ26" s="23"/>
+      <c r="CR26" s="23"/>
+    </row>
+    <row r="27" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A27" s="21">
+        <v>10</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21">
+        <v>8</v>
+      </c>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21">
+        <v>0</v>
+      </c>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21">
+        <v>3</v>
+      </c>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21">
+        <v>19</v>
+      </c>
+      <c r="U27" s="21"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="21"/>
+      <c r="Y27" s="21">
+        <v>21</v>
+      </c>
+      <c r="Z27" s="21"/>
+      <c r="AA27" s="21"/>
+      <c r="AB27" s="21"/>
+      <c r="AC27" s="21"/>
+      <c r="AD27" s="21">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="21"/>
+      <c r="AF27" s="21"/>
+      <c r="AG27">
+        <f>AN25</f>
+        <v>1</v>
+      </c>
+      <c r="AH27">
+        <f>AM25</f>
+        <v>0</v>
+      </c>
+      <c r="AI27">
+        <f>AL25</f>
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <f>AK25</f>
+        <v>1</v>
+      </c>
+      <c r="AK27">
+        <f>AJ25</f>
+        <v>1</v>
+      </c>
+      <c r="AL27">
+        <f>AI25</f>
+        <v>0</v>
+      </c>
+      <c r="AM27">
+        <f>AH25</f>
+        <v>1</v>
+      </c>
+      <c r="AN27">
+        <f>AG25</f>
+        <v>0</v>
+      </c>
+      <c r="AO27">
+        <f>AV25</f>
+        <v>0</v>
+      </c>
+      <c r="AP27">
+        <f>AU25</f>
+        <v>1</v>
+      </c>
+      <c r="AQ27">
+        <f>AT25</f>
+        <v>1</v>
+      </c>
+      <c r="AR27">
+        <f>AS25</f>
+        <v>0</v>
+      </c>
+      <c r="AS27">
+        <f>AR25</f>
+        <v>1</v>
+      </c>
+      <c r="AT27">
+        <f>AQ25</f>
+        <v>0</v>
+      </c>
+      <c r="AU27">
+        <f>AP25</f>
+        <v>0</v>
+      </c>
+      <c r="AV27">
+        <f>AO25</f>
+        <v>1</v>
+      </c>
+      <c r="AW27">
+        <f>BD25</f>
+        <v>1</v>
+      </c>
+      <c r="AX27">
+        <f>BC25</f>
+        <v>0</v>
+      </c>
+      <c r="AY27">
+        <f>BB25</f>
+        <v>1</v>
+      </c>
+      <c r="AZ27">
+        <f>BA25</f>
+        <v>0</v>
+      </c>
+      <c r="BA27">
+        <f>AZ25</f>
+        <v>0</v>
+      </c>
+      <c r="BB27">
+        <f>AY25</f>
+        <v>1</v>
+      </c>
+      <c r="BC27">
+        <f>AX25</f>
+        <v>1</v>
+      </c>
+      <c r="BD27">
+        <f>AW25</f>
+        <v>0</v>
+      </c>
+      <c r="BE27">
+        <f>BL25</f>
+        <v>0</v>
+      </c>
+      <c r="BF27">
+        <f>BK25</f>
+        <v>1</v>
+      </c>
+      <c r="BG27">
+        <f>BJ25</f>
+        <v>0</v>
+      </c>
+      <c r="BH27">
+        <f>BI25</f>
+        <v>1</v>
+      </c>
+      <c r="BI27">
+        <f>BH25</f>
+        <v>1</v>
+      </c>
+      <c r="BJ27">
+        <f>BG25</f>
+        <v>0</v>
+      </c>
+      <c r="BK27">
+        <f>BF25</f>
+        <v>0</v>
+      </c>
+      <c r="BL27">
+        <f>BE25</f>
+        <v>1</v>
+      </c>
+      <c r="BM27">
+        <f>BT25</f>
+        <v>0</v>
+      </c>
+      <c r="BN27">
+        <f>BS25</f>
+        <v>1</v>
+      </c>
+      <c r="BO27">
+        <f>BR25</f>
+        <v>1</v>
+      </c>
+      <c r="BP27">
+        <f>BQ25</f>
+        <v>0</v>
+      </c>
+      <c r="BQ27">
+        <f>BP25</f>
+        <v>0</v>
+      </c>
+      <c r="BR27">
+        <f>BO25</f>
+        <v>1</v>
+      </c>
+      <c r="BS27">
+        <f>BN25</f>
+        <v>0</v>
+      </c>
+      <c r="BT27">
+        <f>BM25</f>
+        <v>1</v>
+      </c>
+      <c r="BU27">
+        <f>CB25</f>
+        <v>1</v>
+      </c>
+      <c r="BV27">
+        <f>CA25</f>
+        <v>0</v>
+      </c>
+      <c r="BW27">
+        <f>BZ25</f>
+        <v>0</v>
+      </c>
+      <c r="BX27">
+        <f>BY25</f>
+        <v>1</v>
+      </c>
+      <c r="BY27">
+        <f>BX25</f>
+        <v>0</v>
+      </c>
+      <c r="BZ27">
+        <f>BW25</f>
+        <v>1</v>
+      </c>
+      <c r="CA27">
+        <f>BV25</f>
+        <v>1</v>
+      </c>
+      <c r="CB27">
+        <f>BU25</f>
+        <v>0</v>
+      </c>
+      <c r="CC27">
+        <f>CJ25</f>
+        <v>0</v>
+      </c>
+      <c r="CD27">
+        <f>CI25</f>
+        <v>1</v>
+      </c>
+      <c r="CE27">
+        <f>CH25</f>
+        <v>0</v>
+      </c>
+      <c r="CF27">
+        <f>CG25</f>
+        <v>1</v>
+      </c>
+      <c r="CG27">
+        <f>CF25</f>
+        <v>1</v>
+      </c>
+      <c r="CH27">
+        <f>CE25</f>
+        <v>0</v>
+      </c>
+      <c r="CI27">
+        <f>CD25</f>
+        <v>0</v>
+      </c>
+      <c r="CJ27">
+        <f>CC25</f>
+        <v>1</v>
+      </c>
+      <c r="CK27">
+        <f>CR25</f>
+        <v>0</v>
+      </c>
+      <c r="CL27">
+        <f>CQ25</f>
+        <v>1</v>
+      </c>
+      <c r="CM27">
+        <f>CP25</f>
+        <v>1</v>
+      </c>
+      <c r="CN27">
+        <f>CO25</f>
+        <v>0</v>
+      </c>
+      <c r="CO27">
+        <f>CN25</f>
+        <v>0</v>
+      </c>
+      <c r="CP27">
+        <f>CM25</f>
+        <v>0</v>
+      </c>
+      <c r="CQ27">
+        <f>CL25</f>
+        <v>0</v>
+      </c>
+      <c r="CR27">
+        <f>CK25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A28" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="R28" s="21"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="U28" s="21"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="21"/>
+      <c r="X28" s="21"/>
+      <c r="Y28" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z28" s="21"/>
+      <c r="AA28" s="21"/>
+      <c r="AB28" s="21"/>
+      <c r="AC28" s="21"/>
+      <c r="AD28" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE28" s="21"/>
+      <c r="AF28" s="21"/>
+      <c r="AG28" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH28" s="23"/>
+      <c r="AI28" s="23"/>
+      <c r="AJ28" s="23"/>
+      <c r="AK28" s="23"/>
+      <c r="AL28" s="23"/>
+      <c r="AM28" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN28" s="23"/>
+      <c r="AO28" s="23"/>
+      <c r="AP28" s="23"/>
+      <c r="AQ28" s="23"/>
+      <c r="AR28" s="23"/>
+      <c r="AS28" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT28" s="23"/>
+      <c r="AU28" s="23"/>
+      <c r="AV28" s="23"/>
+      <c r="AW28" s="23"/>
+      <c r="AX28" s="23"/>
+      <c r="AY28" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ28" s="23"/>
+      <c r="BA28" s="23"/>
+      <c r="BB28" s="23"/>
+      <c r="BC28" s="23"/>
+      <c r="BD28" s="23"/>
+      <c r="BE28" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="BF28" s="23"/>
+      <c r="BG28" s="23"/>
+      <c r="BH28" s="23"/>
+      <c r="BI28" s="23"/>
+      <c r="BJ28" s="23"/>
+      <c r="BK28" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="BL28" s="23"/>
+      <c r="BM28" s="23"/>
+      <c r="BN28" s="23"/>
+      <c r="BO28" s="23"/>
+      <c r="BP28" s="23"/>
+      <c r="BQ28" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR28" s="23"/>
+      <c r="BS28" s="23"/>
+      <c r="BT28" s="23"/>
+      <c r="BU28" s="23"/>
+      <c r="BV28" s="23"/>
+      <c r="BW28" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="BX28" s="23"/>
+      <c r="BY28" s="23"/>
+      <c r="BZ28" s="23"/>
+      <c r="CA28" s="23"/>
+      <c r="CB28" s="23"/>
+      <c r="CC28" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="CD28" s="23"/>
+      <c r="CE28" s="23"/>
+      <c r="CF28" s="23"/>
+      <c r="CG28" s="23"/>
+      <c r="CH28" s="23"/>
+      <c r="CI28" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="CJ28" s="23"/>
+      <c r="CK28" s="23"/>
+      <c r="CL28" s="23"/>
+      <c r="CM28" s="23"/>
+      <c r="CN28" s="23"/>
+    </row>
+    <row r="29" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="A29" s="21">
+        <f>A27</f>
+        <v>10</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="22">
+        <f>100/(2^5-1)*I27</f>
+        <v>25.806451612903224</v>
+      </c>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="23" t="str">
+        <f>LOOKUP(N27,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$18)</f>
+        <v>no error</v>
+      </c>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="24">
+        <f>100/(2^3-1)*Q27</f>
+        <v>42.857142857142861</v>
+      </c>
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24">
+        <f>'Data package'!$B$27*T27+'Data package'!$B$24</f>
+        <v>22.903225806451616</v>
+      </c>
+      <c r="U29" s="23"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
+      <c r="Y29" s="23">
+        <f>Y27</f>
+        <v>21</v>
+      </c>
+      <c r="Z29" s="23"/>
+      <c r="AA29" s="23"/>
+      <c r="AB29" s="23"/>
+      <c r="AC29" s="23"/>
+      <c r="AD29" s="23">
+        <f>LOOKUP(AD27,'Data package'!$A$64:$A$68,'Data package'!$B$64:$B$68)</f>
+        <v>1</v>
+      </c>
+      <c r="AE29" s="23"/>
+      <c r="AF29" s="23"/>
+      <c r="AG29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH29" s="23"/>
+      <c r="AI29" s="23"/>
+      <c r="AJ29" s="23"/>
+      <c r="AK29" s="23"/>
+      <c r="AL29" s="23"/>
+      <c r="AM29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN29" s="23"/>
+      <c r="AO29" s="23"/>
+      <c r="AP29" s="23"/>
+      <c r="AQ29" s="23"/>
+      <c r="AR29" s="23"/>
+      <c r="AS29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT29" s="23"/>
+      <c r="AU29" s="23"/>
+      <c r="AV29" s="23"/>
+      <c r="AW29" s="23"/>
+      <c r="AX29" s="23"/>
+      <c r="AY29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AZ29" s="23"/>
+      <c r="BA29" s="23"/>
+      <c r="BB29" s="23"/>
+      <c r="BC29" s="23"/>
+      <c r="BD29" s="23"/>
+      <c r="BE29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="BF29" s="23"/>
+      <c r="BG29" s="23"/>
+      <c r="BH29" s="23"/>
+      <c r="BI29" s="23"/>
+      <c r="BJ29" s="23"/>
+      <c r="BK29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="BL29" s="23"/>
+      <c r="BM29" s="23"/>
+      <c r="BN29" s="23"/>
+      <c r="BO29" s="23"/>
+      <c r="BP29" s="23"/>
+      <c r="BQ29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="BR29" s="23"/>
+      <c r="BS29" s="23"/>
+      <c r="BT29" s="23"/>
+      <c r="BU29" s="23"/>
+      <c r="BV29" s="23"/>
+      <c r="BW29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="BX29" s="23"/>
+      <c r="BY29" s="23"/>
+      <c r="BZ29" s="23"/>
+      <c r="CA29" s="23"/>
+      <c r="CB29" s="23"/>
+      <c r="CC29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="CD29" s="23"/>
+      <c r="CE29" s="23"/>
+      <c r="CF29" s="23"/>
+      <c r="CG29" s="23"/>
+      <c r="CH29" s="23"/>
+      <c r="CI29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="CJ29" s="23"/>
+      <c r="CK29" s="23"/>
+      <c r="CL29" s="23"/>
+      <c r="CM29" s="23"/>
+      <c r="CN29" s="23"/>
+    </row>
+    <row r="30" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="AG30">
+        <f>AL27</f>
+        <v>0</v>
+      </c>
+      <c r="AH30">
+        <f>AK27</f>
+        <v>1</v>
+      </c>
+      <c r="AI30">
+        <f>AJ27</f>
+        <v>1</v>
+      </c>
+      <c r="AJ30">
+        <f>AI27</f>
+        <v>0</v>
+      </c>
+      <c r="AK30">
+        <f>AH27</f>
+        <v>0</v>
+      </c>
+      <c r="AL30">
+        <f>AG27</f>
+        <v>1</v>
+      </c>
+      <c r="AM30">
+        <f>AR27</f>
+        <v>0</v>
+      </c>
+      <c r="AN30">
+        <f>AQ27</f>
+        <v>1</v>
+      </c>
+      <c r="AO30">
+        <f>AP27</f>
+        <v>1</v>
+      </c>
+      <c r="AP30">
+        <f>AO27</f>
+        <v>0</v>
+      </c>
+      <c r="AQ30">
+        <f>AN27</f>
+        <v>0</v>
+      </c>
+      <c r="AR30">
+        <f>AM27</f>
+        <v>1</v>
+      </c>
+      <c r="AS30">
+        <f>AX27</f>
+        <v>0</v>
+      </c>
+      <c r="AT30">
+        <f>AW27</f>
+        <v>1</v>
+      </c>
+      <c r="AU30">
+        <f>AV27</f>
+        <v>1</v>
+      </c>
+      <c r="AV30">
+        <f>AU27</f>
+        <v>0</v>
+      </c>
+      <c r="AW30">
+        <f>AT27</f>
+        <v>0</v>
+      </c>
+      <c r="AX30">
+        <f>AS27</f>
+        <v>1</v>
+      </c>
+      <c r="AY30">
+        <f>BD27</f>
+        <v>0</v>
+      </c>
+      <c r="AZ30">
+        <f>BC27</f>
+        <v>1</v>
+      </c>
+      <c r="BA30">
+        <f>BB27</f>
+        <v>1</v>
+      </c>
+      <c r="BB30">
+        <f>BA27</f>
+        <v>0</v>
+      </c>
+      <c r="BC30">
+        <f>AZ27</f>
+        <v>0</v>
+      </c>
+      <c r="BD30">
+        <f>AY27</f>
+        <v>1</v>
+      </c>
+      <c r="BE30">
+        <f>BJ27</f>
+        <v>0</v>
+      </c>
+      <c r="BF30">
+        <f>BI27</f>
+        <v>1</v>
+      </c>
+      <c r="BG30">
+        <f>BH27</f>
+        <v>1</v>
+      </c>
+      <c r="BH30">
+        <f>BG27</f>
+        <v>0</v>
+      </c>
+      <c r="BI30">
+        <f>BF27</f>
+        <v>1</v>
+      </c>
+      <c r="BJ30">
+        <f>BE27</f>
+        <v>0</v>
+      </c>
+      <c r="BK30">
+        <f>BP27</f>
+        <v>0</v>
+      </c>
+      <c r="BL30">
+        <f>BO27</f>
+        <v>1</v>
+      </c>
+      <c r="BM30">
+        <f>BN27</f>
+        <v>1</v>
+      </c>
+      <c r="BN30">
+        <f>BM27</f>
+        <v>0</v>
+      </c>
+      <c r="BO30">
+        <f>BL27</f>
+        <v>1</v>
+      </c>
+      <c r="BP30">
+        <f>BK27</f>
+        <v>0</v>
+      </c>
+      <c r="BQ30">
+        <f>BV27</f>
+        <v>0</v>
+      </c>
+      <c r="BR30">
+        <f>BU27</f>
+        <v>1</v>
+      </c>
+      <c r="BS30">
+        <f>BT27</f>
+        <v>1</v>
+      </c>
+      <c r="BT30">
+        <f>BS27</f>
+        <v>0</v>
+      </c>
+      <c r="BU30">
+        <f>BR27</f>
+        <v>1</v>
+      </c>
+      <c r="BV30">
+        <f>BQ27</f>
+        <v>0</v>
+      </c>
+      <c r="BW30">
+        <f>CB27</f>
+        <v>0</v>
+      </c>
+      <c r="BX30">
+        <f>CA27</f>
+        <v>1</v>
+      </c>
+      <c r="BY30">
+        <f>BZ27</f>
+        <v>1</v>
+      </c>
+      <c r="BZ30">
+        <f>BY27</f>
+        <v>0</v>
+      </c>
+      <c r="CA30">
+        <f>BX27</f>
+        <v>1</v>
+      </c>
+      <c r="CB30">
+        <f>BW27</f>
+        <v>0</v>
+      </c>
+      <c r="CC30">
+        <f>CH27</f>
+        <v>0</v>
+      </c>
+      <c r="CD30">
+        <f>CG27</f>
+        <v>1</v>
+      </c>
+      <c r="CE30">
+        <f>CF27</f>
+        <v>1</v>
+      </c>
+      <c r="CF30">
+        <f>CE27</f>
+        <v>0</v>
+      </c>
+      <c r="CG30">
+        <f>CD27</f>
+        <v>1</v>
+      </c>
+      <c r="CH30">
+        <f>CC27</f>
+        <v>0</v>
+      </c>
+      <c r="CI30">
+        <f>CN27</f>
+        <v>0</v>
+      </c>
+      <c r="CJ30">
+        <f>CM27</f>
+        <v>1</v>
+      </c>
+      <c r="CK30">
+        <f>CL27</f>
+        <v>1</v>
+      </c>
+      <c r="CL30">
+        <f>CK27</f>
+        <v>0</v>
+      </c>
+      <c r="CM30">
+        <f>CJ27</f>
+        <v>1</v>
+      </c>
+      <c r="CN30">
+        <f>CI27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="AG31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH31" s="23"/>
+      <c r="AI31" s="23"/>
+      <c r="AJ31" s="23"/>
+      <c r="AK31" s="23"/>
+      <c r="AL31" s="23"/>
+      <c r="AM31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN31" s="23"/>
+      <c r="AO31" s="23"/>
+      <c r="AP31" s="23"/>
+      <c r="AQ31" s="23"/>
+      <c r="AR31" s="23"/>
+      <c r="AS31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AT31" s="23"/>
+      <c r="AU31" s="23"/>
+      <c r="AV31" s="23"/>
+      <c r="AW31" s="23"/>
+      <c r="AX31" s="23"/>
+      <c r="AY31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="AZ31" s="23"/>
+      <c r="BA31" s="23"/>
+      <c r="BB31" s="23"/>
+      <c r="BC31" s="23"/>
+      <c r="BD31" s="23"/>
+      <c r="BE31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="BF31" s="23"/>
+      <c r="BG31" s="23"/>
+      <c r="BH31" s="23"/>
+      <c r="BI31" s="23"/>
+      <c r="BJ31" s="23"/>
+      <c r="BK31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="BL31" s="23"/>
+      <c r="BM31" s="23"/>
+      <c r="BN31" s="23"/>
+      <c r="BO31" s="23"/>
+      <c r="BP31" s="23"/>
+      <c r="BQ31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="BR31" s="23"/>
+      <c r="BS31" s="23"/>
+      <c r="BT31" s="23"/>
+      <c r="BU31" s="23"/>
+      <c r="BV31" s="23"/>
+      <c r="BW31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="BX31" s="23"/>
+      <c r="BY31" s="23"/>
+      <c r="BZ31" s="23"/>
+      <c r="CA31" s="23"/>
+      <c r="CB31" s="23"/>
+      <c r="CC31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="CD31" s="23"/>
+      <c r="CE31" s="23"/>
+      <c r="CF31" s="23"/>
+      <c r="CG31" s="23"/>
+      <c r="CH31" s="23"/>
+      <c r="CI31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="CJ31" s="23"/>
+      <c r="CK31" s="23"/>
+      <c r="CL31" s="23"/>
+      <c r="CM31" s="23"/>
+      <c r="CN31" s="23"/>
+    </row>
+    <row r="32" spans="1:96" x14ac:dyDescent="0.3">
+      <c r="AG32" s="23">
+        <v>25</v>
+      </c>
+      <c r="AH32" s="23"/>
+      <c r="AI32" s="23"/>
+      <c r="AJ32" s="23"/>
+      <c r="AK32" s="23"/>
+      <c r="AL32" s="23"/>
+      <c r="AM32" s="23">
+        <v>25</v>
+      </c>
+      <c r="AN32" s="23"/>
+      <c r="AO32" s="23"/>
+      <c r="AP32" s="23"/>
+      <c r="AQ32" s="23"/>
+      <c r="AR32" s="23"/>
+      <c r="AS32" s="23">
+        <v>25</v>
+      </c>
+      <c r="AT32" s="23"/>
+      <c r="AU32" s="23"/>
+      <c r="AV32" s="23"/>
+      <c r="AW32" s="23"/>
+      <c r="AX32" s="23"/>
+      <c r="AY32" s="23">
+        <v>25</v>
+      </c>
+      <c r="AZ32" s="23"/>
+      <c r="BA32" s="23"/>
+      <c r="BB32" s="23"/>
+      <c r="BC32" s="23"/>
+      <c r="BD32" s="23"/>
+      <c r="BE32" s="23">
+        <v>26</v>
+      </c>
+      <c r="BF32" s="23"/>
+      <c r="BG32" s="23"/>
+      <c r="BH32" s="23"/>
+      <c r="BI32" s="23"/>
+      <c r="BJ32" s="23"/>
+      <c r="BK32" s="23">
+        <v>26</v>
+      </c>
+      <c r="BL32" s="23"/>
+      <c r="BM32" s="23"/>
+      <c r="BN32" s="23"/>
+      <c r="BO32" s="23"/>
+      <c r="BP32" s="23"/>
+      <c r="BQ32" s="23">
+        <v>26</v>
+      </c>
+      <c r="BR32" s="23"/>
+      <c r="BS32" s="23"/>
+      <c r="BT32" s="23"/>
+      <c r="BU32" s="23"/>
+      <c r="BV32" s="23"/>
+      <c r="BW32" s="23">
+        <v>26</v>
+      </c>
+      <c r="BX32" s="23"/>
+      <c r="BY32" s="23"/>
+      <c r="BZ32" s="23"/>
+      <c r="CA32" s="23"/>
+      <c r="CB32" s="23"/>
+      <c r="CC32" s="23">
+        <v>26</v>
+      </c>
+      <c r="CD32" s="23"/>
+      <c r="CE32" s="23"/>
+      <c r="CF32" s="23"/>
+      <c r="CG32" s="23"/>
+      <c r="CH32" s="23"/>
+      <c r="CI32" s="23">
+        <v>26</v>
+      </c>
+      <c r="CJ32" s="23"/>
+      <c r="CK32" s="23"/>
+      <c r="CL32" s="23"/>
+      <c r="CM32" s="23"/>
+      <c r="CN32" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="77">
+  <mergeCells count="166">
+    <mergeCell ref="BK32:BP32"/>
+    <mergeCell ref="BQ32:BV32"/>
+    <mergeCell ref="BW32:CB32"/>
+    <mergeCell ref="CC32:CH32"/>
+    <mergeCell ref="CI32:CN32"/>
+    <mergeCell ref="AG32:AL32"/>
+    <mergeCell ref="AM32:AR32"/>
+    <mergeCell ref="AS32:AX32"/>
+    <mergeCell ref="AY32:BD32"/>
+    <mergeCell ref="BE32:BJ32"/>
+    <mergeCell ref="BK31:BP31"/>
+    <mergeCell ref="BQ31:BV31"/>
+    <mergeCell ref="BW31:CB31"/>
+    <mergeCell ref="CC31:CH31"/>
+    <mergeCell ref="CI31:CN31"/>
+    <mergeCell ref="AG31:AL31"/>
+    <mergeCell ref="AM31:AR31"/>
+    <mergeCell ref="AS31:AX31"/>
+    <mergeCell ref="AY31:BD31"/>
+    <mergeCell ref="BE31:BJ31"/>
+    <mergeCell ref="BK29:BP29"/>
+    <mergeCell ref="BQ29:BV29"/>
+    <mergeCell ref="BW29:CB29"/>
+    <mergeCell ref="CC29:CH29"/>
+    <mergeCell ref="CI29:CN29"/>
+    <mergeCell ref="AG29:AL29"/>
+    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AS29:AX29"/>
+    <mergeCell ref="AY29:BD29"/>
+    <mergeCell ref="BE29:BJ29"/>
+    <mergeCell ref="BK28:BP28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="BW28:CB28"/>
+    <mergeCell ref="CC28:CH28"/>
+    <mergeCell ref="CI28:CN28"/>
+    <mergeCell ref="AG28:AL28"/>
+    <mergeCell ref="AM28:AR28"/>
+    <mergeCell ref="AS28:AX28"/>
+    <mergeCell ref="AY28:BD28"/>
+    <mergeCell ref="BE28:BJ28"/>
+    <mergeCell ref="BU24:CB24"/>
+    <mergeCell ref="CC24:CJ24"/>
+    <mergeCell ref="CK24:CR24"/>
+    <mergeCell ref="AG26:AN26"/>
+    <mergeCell ref="AO26:AV26"/>
+    <mergeCell ref="AW26:BD26"/>
+    <mergeCell ref="BE26:BL26"/>
+    <mergeCell ref="BM26:BT26"/>
+    <mergeCell ref="BU26:CB26"/>
+    <mergeCell ref="CC26:CJ26"/>
+    <mergeCell ref="CK26:CR26"/>
+    <mergeCell ref="AG24:AN24"/>
+    <mergeCell ref="AO24:AV24"/>
+    <mergeCell ref="AW24:BD24"/>
+    <mergeCell ref="BE24:BL24"/>
+    <mergeCell ref="BM24:BT24"/>
+    <mergeCell ref="Y28:AC28"/>
+    <mergeCell ref="AD28:AF28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="Y26:AC26"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:X27"/>
+    <mergeCell ref="Y27:AC27"/>
+    <mergeCell ref="AD27:AF27"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="A23:AF23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="I24:P24"/>
+    <mergeCell ref="Q24:X24"/>
+    <mergeCell ref="Y24:AF24"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="Q1:X1"/>
+    <mergeCell ref="Y1:AF1"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="AD3:AF3"/>
+    <mergeCell ref="Y3:AC3"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="A5:AF5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="I6:P6"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="Y6:AF6"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="T9:X9"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="Q15:X15"/>
+    <mergeCell ref="Y15:AF15"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T17:X17"/>
     <mergeCell ref="Y19:AC19"/>
     <mergeCell ref="AD19:AF19"/>
     <mergeCell ref="A20:H20"/>
@@ -3633,69 +5389,6 @@
     <mergeCell ref="N19:P19"/>
     <mergeCell ref="Q19:S19"/>
     <mergeCell ref="T19:X19"/>
-    <mergeCell ref="Y17:AC17"/>
-    <mergeCell ref="AD17:AF17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="Y18:AC18"/>
-    <mergeCell ref="AD18:AF18"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="I15:P15"/>
-    <mergeCell ref="Q15:X15"/>
-    <mergeCell ref="Y15:AF15"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="Y10:AC10"/>
-    <mergeCell ref="T10:X10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="Y11:AC11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="T9:X9"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="Y6:AF6"/>
-    <mergeCell ref="AD9:AF9"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="Y9:AC9"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="A5:AF5"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="I6:P6"/>
-    <mergeCell ref="I8:M8"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:P1"/>
-    <mergeCell ref="Q1:X1"/>
-    <mergeCell ref="Y1:AF1"/>
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="AD3:AF3"/>
-    <mergeCell ref="Y3:AC3"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3724,44 +5417,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="11">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="K3" s="29" t="s">
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="K3" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29" t="s">
+      <c r="L3" s="36"/>
+      <c r="M3" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="12">
         <v>0.01</v>
       </c>
@@ -3780,8 +5473,8 @@
       <c r="I4" s="12">
         <v>10</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
       <c r="M4" s="12">
         <v>0.01</v>
       </c>
@@ -3802,7 +5495,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="37" t="s">
         <v>42</v>
       </c>
       <c r="C5" s="12">
@@ -3832,7 +5525,7 @@
         <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="37" t="s">
         <v>42</v>
       </c>
       <c r="L5" s="12">
@@ -3864,7 +5557,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="30"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="12">
         <v>0.02</v>
       </c>
@@ -3892,7 +5585,7 @@
         <f t="shared" si="2"/>
         <v>2E-3</v>
       </c>
-      <c r="K6" s="30"/>
+      <c r="K6" s="37"/>
       <c r="L6" s="12">
         <v>0.02</v>
       </c>
@@ -3922,7 +5615,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="30"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="12">
         <v>0.03</v>
       </c>
@@ -3950,7 +5643,7 @@
         <f t="shared" si="2"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K7" s="30"/>
+      <c r="K7" s="37"/>
       <c r="L7" s="12">
         <v>0.03</v>
       </c>
@@ -3980,7 +5673,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="30"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="12">
         <v>0.05</v>
       </c>
@@ -4008,7 +5701,7 @@
         <f t="shared" si="2"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K8" s="30"/>
+      <c r="K8" s="37"/>
       <c r="L8" s="12">
         <v>0.05</v>
       </c>
@@ -4038,7 +5731,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="30"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="12">
         <v>0.1</v>
       </c>
@@ -4066,7 +5759,7 @@
         <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
-      <c r="K9" s="30"/>
+      <c r="K9" s="37"/>
       <c r="L9" s="12">
         <v>0.1</v>
       </c>
@@ -4096,7 +5789,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="30"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="12">
         <v>0.2</v>
       </c>
@@ -4124,7 +5817,7 @@
         <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
-      <c r="K10" s="30"/>
+      <c r="K10" s="37"/>
       <c r="L10" s="12">
         <v>0.2</v>
       </c>
@@ -4154,7 +5847,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="30"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="12">
         <v>0.3</v>
       </c>
@@ -4182,7 +5875,7 @@
         <f t="shared" si="2"/>
         <v>0.03</v>
       </c>
-      <c r="K11" s="30"/>
+      <c r="K11" s="37"/>
       <c r="L11" s="12">
         <v>0.3</v>
       </c>
@@ -4212,7 +5905,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="30"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="12">
         <v>0.5</v>
       </c>
@@ -4240,7 +5933,7 @@
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
-      <c r="K12" s="30"/>
+      <c r="K12" s="37"/>
       <c r="L12" s="12">
         <v>0.5</v>
       </c>
@@ -4270,7 +5963,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="30"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="12">
         <v>1</v>
       </c>
@@ -4298,7 +5991,7 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="K13" s="30"/>
+      <c r="K13" s="37"/>
       <c r="L13" s="12">
         <v>1</v>
       </c>
@@ -4478,24 +6171,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
@@ -4554,28 +6247,28 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="25" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="25" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="26"/>
-      <c r="P3" s="27"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="35"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -4631,21 +6324,21 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="28" t="s">
+      <c r="R6" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="28"/>
+      <c r="S6" s="21"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -4683,10 +6376,10 @@
       <c r="Q7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R7" s="33" t="s">
+      <c r="R7" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="S7" s="33"/>
+      <c r="S7" s="38"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
@@ -4697,18 +6390,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28" t="s">
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
@@ -4722,18 +6415,18 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="28">
+      <c r="I9" s="21">
         <v>17</v>
       </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28">
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21">
         <v>4</v>
       </c>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
@@ -4752,11 +6445,11 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="28" t="s">
+      <c r="N10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -4775,18 +6468,24 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="32">
+      <c r="N11" s="22">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -4794,12 +6493,6 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Battery level changed to battery voltage in data package
</commit_message>
<xml_diff>
--- a/hardware/DataPackage.xlsx
+++ b/hardware/DataPackage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\Repos\lora\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F0268F-2BFF-4595-83FC-F7B8E56D10B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797A9CEF-76B0-4804-BB36-33C2CC6CBE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15636" yWindow="156" windowWidth="25644" windowHeight="15960" activeTab="1" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
+    <workbookView xWindow="41172" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{CDF7A0A5-12B1-43F1-AFDE-54CA91221B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Data package" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="88">
   <si>
     <t>minutes of day</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Temperatur</t>
   </si>
   <si>
-    <t>Battery level</t>
-  </si>
-  <si>
     <t>Humidity</t>
   </si>
   <si>
@@ -214,9 +211,6 @@
     <t>Index</t>
   </si>
   <si>
-    <t>Battery Level [%]</t>
-  </si>
-  <si>
     <t>Humidity [%]</t>
   </si>
   <si>
@@ -290,14 +284,33 @@
   </si>
   <si>
     <t>min. of hour</t>
+  </si>
+  <si>
+    <t>Battery voltage</t>
+  </si>
+  <si>
+    <t>min. Voltage [V]</t>
+  </si>
+  <si>
+    <t>max. Voltage [V]</t>
+  </si>
+  <si>
+    <t>dV [V]</t>
+  </si>
+  <si>
+    <t>BatteryVoltage</t>
+  </si>
+  <si>
+    <t>Battery Voltage [V]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -492,7 +505,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -545,21 +558,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -598,9 +614,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -2048,10 +2062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088FF0E6-8FE4-49E3-812F-B76B934E1ACD}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2118,7 +2132,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2157,7 +2171,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="D16">
         <v>5</v>
@@ -2176,11 +2190,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="2">
-        <f>100/(2^B17-1)</f>
-        <v>3.225806451612903</v>
+        <v>83</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
       </c>
       <c r="D18">
         <v>7</v>
@@ -2188,498 +2201,524 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20">
+        <f>B19-B18</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="40">
+        <f>B20/(2^B17-1)</f>
+        <v>4.8387096774193547E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B22" s="4">
         <f>B13-B17</f>
         <v>392</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24">
-        <v>-20</v>
-      </c>
-    </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B26">
-        <f>B25-B24</f>
-        <v>70</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="2">
-        <f>B26/(2^B23-1)</f>
-        <v>2.2580645161290325</v>
-      </c>
-      <c r="D27" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="B27">
+        <v>-20</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="4">
-        <f>B19-B23</f>
-        <v>387</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <f>B28-B27</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="2">
+        <f>B29/(2^B26-1)</f>
+        <v>2.2580645161290325</v>
+      </c>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="2">
-        <f>100/(2^B32-1)</f>
-        <v>14.285714285714286</v>
+        <v>18</v>
+      </c>
+      <c r="B31" s="4">
+        <f>B22-B26</f>
+        <v>387</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="4">
-        <f>B28-B32</f>
-        <v>384</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="2">
+        <f>100/(2^B35-1)</f>
+        <v>14.285714285714286</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="4">
+        <f>B31-B35</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>11</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="4">
-        <f>B34-B38</f>
+      <c r="B42" s="4">
+        <f>B37-B41</f>
         <v>384</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="20" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46">
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49">
         <v>1440</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C49" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="3">
-        <f>B39/B47</f>
+      <c r="D49" s="3">
+        <f>B42/B50</f>
         <v>34.909090909090907</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>2</v>
       </c>
-      <c r="B47">
+      <c r="B50">
         <v>11</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C50" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="14">
-        <f>ROUNDDOWN(D46,0)</f>
+      <c r="D50" s="14">
+        <f>ROUNDDOWN(D49,0)</f>
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B48">
-        <f>2^B47</f>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <f>2^B50</f>
         <v>2048</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C51" t="s">
         <v>18</v>
       </c>
-      <c r="D48">
-        <f>B39-D47*B47</f>
+      <c r="D51">
+        <f>B42-D50*B50</f>
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="20" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B54" s="13">
-        <v>3</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B55" s="17">
-        <f>B39-B54</f>
-        <v>381</v>
-      </c>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" s="13"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" s="1"/>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="13">
+        <v>3</v>
+      </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B58" s="1">
-        <v>5</v>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="17">
+        <f>B42-B57</f>
+        <v>381</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B59" s="1">
-        <f>2^B58</f>
-        <v>32</v>
-      </c>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B61" s="6">
-        <f>B55-B58</f>
-        <v>376</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D61" s="1">
-        <f>B61/8</f>
-        <v>47</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B61" s="1">
+        <v>5</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" s="1">
+        <f>2^B61</f>
+        <v>32</v>
+      </c>
+      <c r="C62" s="1"/>
       <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" s="6">
+        <f>B58-B61</f>
+        <v>376</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" s="1">
+        <f>B64/8</f>
+        <v>47</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" t="s">
+        <v>3</v>
+      </c>
+      <c r="G66" t="s">
+        <v>19</v>
+      </c>
+      <c r="H66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <f>B67*60</f>
+        <v>60</v>
+      </c>
+      <c r="D67">
+        <v>6</v>
+      </c>
+      <c r="E67">
+        <f>2^D67</f>
+        <v>64</v>
+      </c>
+      <c r="F67" s="3">
+        <f>$B$64/D67</f>
+        <v>62.666666666666664</v>
+      </c>
+      <c r="G67" s="5">
+        <f>ROUNDDOWN(F67,0)</f>
+        <v>62</v>
+      </c>
+      <c r="H67">
+        <f t="shared" ref="H67:H69" si="0">$B$64-G67*D67</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ref="C68:C71" si="1">B68*60</f>
+        <v>120</v>
+      </c>
+      <c r="D68">
+        <v>7</v>
+      </c>
+      <c r="E68">
+        <f t="shared" ref="E68:E71" si="2">2^D68</f>
+        <v>128</v>
+      </c>
+      <c r="F68" s="3">
+        <f>$B$64/D68</f>
+        <v>53.714285714285715</v>
+      </c>
+      <c r="G68" s="5">
+        <f t="shared" ref="G68:G71" si="3">ROUNDDOWN(F68,0)</f>
         <v>53</v>
       </c>
-      <c r="B63" t="s">
-        <v>9</v>
-      </c>
-      <c r="C63" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" t="s">
-        <v>6</v>
-      </c>
-      <c r="F63" t="s">
-        <v>3</v>
-      </c>
-      <c r="G63" t="s">
-        <v>19</v>
-      </c>
-      <c r="H63" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <v>0</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64">
-        <f>B64*60</f>
-        <v>60</v>
-      </c>
-      <c r="D64">
-        <v>6</v>
-      </c>
-      <c r="E64">
-        <f>2^D64</f>
-        <v>64</v>
-      </c>
-      <c r="F64" s="3">
-        <f>$B$61/D64</f>
-        <v>62.666666666666664</v>
-      </c>
-      <c r="G64" s="5">
-        <f>ROUNDDOWN(F64,0)</f>
-        <v>62</v>
-      </c>
-      <c r="H64">
-        <f t="shared" ref="H64:H66" si="0">$B$61-G64*D64</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <v>1</v>
-      </c>
-      <c r="B65">
-        <v>2</v>
-      </c>
-      <c r="C65">
-        <f t="shared" ref="C65:C68" si="1">B65*60</f>
-        <v>120</v>
-      </c>
-      <c r="D65">
-        <v>7</v>
-      </c>
-      <c r="E65">
-        <f t="shared" ref="E65:E68" si="2">2^D65</f>
-        <v>128</v>
-      </c>
-      <c r="F65" s="3">
-        <f>$B$61/D65</f>
-        <v>53.714285714285715</v>
-      </c>
-      <c r="G65" s="5">
-        <f t="shared" ref="G65:G68" si="3">ROUNDDOWN(F65,0)</f>
-        <v>53</v>
-      </c>
-      <c r="H65">
+      <c r="H68">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69">
         <v>2</v>
       </c>
-      <c r="B66">
+      <c r="B69">
         <v>4</v>
       </c>
-      <c r="C66">
+      <c r="C69">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="D66">
+      <c r="D69">
         <v>8</v>
       </c>
-      <c r="E66">
+      <c r="E69">
         <f t="shared" si="2"/>
         <v>256</v>
       </c>
-      <c r="F66" s="3">
-        <f>$B$61/D66</f>
+      <c r="F69" s="3">
+        <f>$B$64/D69</f>
         <v>47</v>
       </c>
-      <c r="G66" s="5">
+      <c r="G69" s="5">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="H66">
+      <c r="H69">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70">
         <v>3</v>
       </c>
-      <c r="B67">
+      <c r="B70">
         <v>8</v>
       </c>
-      <c r="C67">
+      <c r="C70">
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="D67">
+      <c r="D70">
         <v>9</v>
       </c>
-      <c r="E67">
+      <c r="E70">
         <f t="shared" si="2"/>
         <v>512</v>
       </c>
-      <c r="F67" s="3">
-        <f>$B$61/D67</f>
+      <c r="F70" s="3">
+        <f>$B$64/D70</f>
         <v>41.777777777777779</v>
       </c>
-      <c r="G67" s="5">
+      <c r="G70" s="5">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="H67">
-        <f>$B$61-G67*D67</f>
+      <c r="H70">
+        <f>$B$64-G70*D70</f>
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71">
         <v>4</v>
       </c>
-      <c r="B68">
+      <c r="B71">
         <v>17</v>
       </c>
-      <c r="C68">
+      <c r="C71">
         <f t="shared" si="1"/>
         <v>1020</v>
       </c>
-      <c r="D68">
+      <c r="D71">
         <v>10</v>
       </c>
-      <c r="E68">
+      <c r="E71">
         <f t="shared" si="2"/>
         <v>1024</v>
       </c>
-      <c r="F68" s="3">
-        <f>$B$61/D68</f>
+      <c r="F71" s="3">
+        <f>$B$64/D71</f>
         <v>37.6</v>
       </c>
-      <c r="G68" s="5">
+      <c r="G71" s="5">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="H68">
-        <f>$B$61-G68*D68</f>
+      <c r="H71">
+        <f>$B$64-G71*D71</f>
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E69" s="3"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E70" s="3"/>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E73" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A54:F54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2690,8 +2729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8852597E-F5BB-40E1-97DB-5D341DB313BD}">
   <dimension ref="A1:CR32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK17" sqref="AK17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2701,46 +2740,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="27" t="s">
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="30"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -2841,52 +2880,52 @@
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="34"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" s="34"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="30" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="35"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="35"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-      <c r="W3" s="31"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="30" t="s">
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="33"/>
+      <c r="Y3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="31"/>
-      <c r="AA3" s="31"/>
-      <c r="AB3" s="31"/>
-      <c r="AC3" s="32"/>
-      <c r="AD3" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE3" s="31"/>
-      <c r="AF3" s="32"/>
+      <c r="Z3" s="32"/>
+      <c r="AA3" s="32"/>
+      <c r="AB3" s="32"/>
+      <c r="AC3" s="33"/>
+      <c r="AD3" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE3" s="32"/>
+      <c r="AF3" s="33"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
@@ -2946,46 +2985,46 @@
       <c r="AF5" s="26"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25">
+      <c r="A6" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27">
         <v>38</v>
       </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25">
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27">
         <v>73</v>
       </c>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25">
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="27">
         <v>88</v>
       </c>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="25"/>
-      <c r="AE6" s="25"/>
-      <c r="AF6" s="25"/>
+      <c r="Z6" s="27"/>
+      <c r="AA6" s="27"/>
+      <c r="AB6" s="27"/>
+      <c r="AC6" s="27"/>
+      <c r="AD6" s="27"/>
+      <c r="AE6" s="27"/>
+      <c r="AF6" s="27"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
@@ -3086,203 +3125,203 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21" t="s">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21" t="s">
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21" t="s">
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21" t="s">
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21" t="s">
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21" t="s">
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="AE8" s="21"/>
-      <c r="AF8" s="21"/>
+      <c r="AE8" s="23"/>
+      <c r="AF8" s="23"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="21">
+      <c r="A9" s="23">
         <v>10</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23">
         <v>7</v>
       </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21">
-        <v>0</v>
-      </c>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21">
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23">
+        <v>0</v>
+      </c>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23">
         <v>3</v>
       </c>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21">
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23">
         <v>19</v>
       </c>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21">
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="23">
         <v>17</v>
       </c>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="21"/>
-      <c r="AF9" s="21"/>
+      <c r="Z9" s="23"/>
+      <c r="AA9" s="23"/>
+      <c r="AB9" s="23"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="23">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="23"/>
+      <c r="AF9" s="23"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21" t="s">
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21" t="s">
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="23"/>
+      <c r="Y10" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21" t="s">
+      <c r="Z10" s="23"/>
+      <c r="AA10" s="23"/>
+      <c r="AB10" s="23"/>
+      <c r="AC10" s="23"/>
+      <c r="AD10" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="21"/>
-      <c r="AD10" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE10" s="21"/>
-      <c r="AF10" s="21"/>
+      <c r="AE10" s="23"/>
+      <c r="AF10" s="23"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="21">
+      <c r="A11" s="23">
         <f>A9</f>
         <v>10</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="22">
-        <f>100/(2^5-1)*I9</f>
-        <v>22.58064516129032</v>
-      </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="23" t="str">
-        <f>LOOKUP(N9,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$18)</f>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24">
+        <f>'Data package'!$B$21*I9+'Data package'!$B$18</f>
+        <v>3.338709677419355</v>
+      </c>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="21" t="str">
+        <f ca="1">LOOKUP(N9,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$21)</f>
         <v>no error</v>
       </c>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="24">
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="25">
         <f>100/(2^3-1)*Q9</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24">
-        <f>'Data package'!$B$27*T9+'Data package'!$B$24</f>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25">
+        <f>'Data package'!$B$30*T9+'Data package'!$B$27</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23">
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21">
         <f>Y9</f>
         <v>17</v>
       </c>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="23">
-        <f>LOOKUP(AD9,'Data package'!$A$64:$A$68,'Data package'!$B$64:$B$68)</f>
-        <v>1</v>
-      </c>
-      <c r="AE11" s="23"/>
-      <c r="AF11" s="23"/>
+      <c r="Z11" s="21"/>
+      <c r="AA11" s="21"/>
+      <c r="AB11" s="21"/>
+      <c r="AC11" s="21"/>
+      <c r="AD11" s="21">
+        <f>LOOKUP(AD9,'Data package'!$A$67:$A$71,'Data package'!$B$67:$B$71)</f>
+        <v>1</v>
+      </c>
+      <c r="AE11" s="21"/>
+      <c r="AF11" s="21"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
@@ -3334,46 +3373,46 @@
       <c r="AF14" s="26"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25" t="s">
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="27"/>
+      <c r="Y15" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25"/>
-      <c r="Y15" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z15" s="25"/>
-      <c r="AA15" s="25"/>
-      <c r="AB15" s="25"/>
-      <c r="AC15" s="25"/>
-      <c r="AD15" s="25"/>
-      <c r="AE15" s="25"/>
-      <c r="AF15" s="25"/>
+      <c r="Z15" s="27"/>
+      <c r="AA15" s="27"/>
+      <c r="AB15" s="27"/>
+      <c r="AC15" s="27"/>
+      <c r="AD15" s="27"/>
+      <c r="AE15" s="27"/>
+      <c r="AF15" s="27"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
@@ -3474,203 +3513,203 @@
       </c>
     </row>
     <row r="17" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21" t="s">
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21" t="s">
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21" t="s">
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="21"/>
-      <c r="Y17" s="21" t="s">
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="21"/>
-      <c r="AA17" s="21"/>
-      <c r="AB17" s="21"/>
-      <c r="AC17" s="21"/>
-      <c r="AD17" s="21" t="s">
+      <c r="Z17" s="23"/>
+      <c r="AA17" s="23"/>
+      <c r="AB17" s="23"/>
+      <c r="AC17" s="23"/>
+      <c r="AD17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="21"/>
-      <c r="AF17" s="21"/>
+      <c r="AE17" s="23"/>
+      <c r="AF17" s="23"/>
     </row>
     <row r="18" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A18" s="21">
+      <c r="A18" s="23">
         <v>5</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23">
         <v>8</v>
       </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21">
-        <v>0</v>
-      </c>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21">
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23">
+        <v>0</v>
+      </c>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23">
         <v>3</v>
       </c>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21">
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23">
         <v>19</v>
       </c>
-      <c r="U18" s="21"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="21"/>
-      <c r="X18" s="21"/>
-      <c r="Y18" s="21">
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="23">
         <v>17</v>
       </c>
-      <c r="Z18" s="21"/>
-      <c r="AA18" s="21"/>
-      <c r="AB18" s="21"/>
-      <c r="AC18" s="21"/>
-      <c r="AD18" s="21">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="21"/>
-      <c r="AF18" s="21"/>
+      <c r="Z18" s="23"/>
+      <c r="AA18" s="23"/>
+      <c r="AB18" s="23"/>
+      <c r="AC18" s="23"/>
+      <c r="AD18" s="23">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="23"/>
+      <c r="AF18" s="23"/>
     </row>
     <row r="19" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21" t="s">
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21" t="s">
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21" t="s">
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="23"/>
+      <c r="AD19" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z19" s="21"/>
-      <c r="AA19" s="21"/>
-      <c r="AB19" s="21"/>
-      <c r="AC19" s="21"/>
-      <c r="AD19" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE19" s="21"/>
-      <c r="AF19" s="21"/>
+      <c r="AE19" s="23"/>
+      <c r="AF19" s="23"/>
     </row>
     <row r="20" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A20" s="21">
+      <c r="A20" s="23">
         <f>A18</f>
         <v>5</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22">
-        <f>100/(2^5-1)*I18</f>
-        <v>25.806451612903224</v>
-      </c>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="23" t="str">
-        <f>LOOKUP(N18,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$18)</f>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="24">
+        <f>'Data package'!$B$21*I18+'Data package'!$B$18</f>
+        <v>3.3870967741935485</v>
+      </c>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="21" t="str">
+        <f ca="1">LOOKUP(N18,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$21)</f>
         <v>no error</v>
       </c>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="24">
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="25">
         <f>100/(2^3-1)*Q18</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24">
-        <f>'Data package'!$B$27*T18+'Data package'!$B$24</f>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25">
+        <f>'Data package'!$B$30*T18+'Data package'!$B$27</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U20" s="23"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="23"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="23">
+      <c r="U20" s="21"/>
+      <c r="V20" s="21"/>
+      <c r="W20" s="21"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="21">
         <f>Y18</f>
         <v>17</v>
       </c>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="23"/>
-      <c r="AB20" s="23"/>
-      <c r="AC20" s="23"/>
-      <c r="AD20" s="23">
-        <f>LOOKUP(AD18,'Data package'!$A$64:$A$68,'Data package'!$B$64:$B$68)</f>
-        <v>1</v>
-      </c>
-      <c r="AE20" s="23"/>
-      <c r="AF20" s="23"/>
+      <c r="Z20" s="21"/>
+      <c r="AA20" s="21"/>
+      <c r="AB20" s="21"/>
+      <c r="AC20" s="21"/>
+      <c r="AD20" s="21">
+        <f>LOOKUP(AD18,'Data package'!$A$67:$A$71,'Data package'!$B$67:$B$71)</f>
+        <v>1</v>
+      </c>
+      <c r="AE20" s="21"/>
+      <c r="AF20" s="21"/>
     </row>
     <row r="23" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
@@ -3709,126 +3748,126 @@
       <c r="AF23" s="26"/>
     </row>
     <row r="24" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25" t="s">
+      <c r="A24" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z24" s="27"/>
+      <c r="AA24" s="27"/>
+      <c r="AB24" s="27"/>
+      <c r="AC24" s="27"/>
+      <c r="AD24" s="27"/>
+      <c r="AE24" s="27"/>
+      <c r="AF24" s="27"/>
+      <c r="AG24" s="22">
+        <v>59</v>
+      </c>
+      <c r="AH24" s="22"/>
+      <c r="AI24" s="22"/>
+      <c r="AJ24" s="22"/>
+      <c r="AK24" s="22"/>
+      <c r="AL24" s="22"/>
+      <c r="AM24" s="22"/>
+      <c r="AN24" s="22"/>
+      <c r="AO24" s="22">
+        <v>96</v>
+      </c>
+      <c r="AP24" s="22"/>
+      <c r="AQ24" s="22"/>
+      <c r="AR24" s="22"/>
+      <c r="AS24" s="22"/>
+      <c r="AT24" s="22"/>
+      <c r="AU24" s="22"/>
+      <c r="AV24" s="22"/>
+      <c r="AW24" s="22">
         <v>65</v>
       </c>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="R24" s="25"/>
-      <c r="S24" s="25"/>
-      <c r="T24" s="25"/>
-      <c r="U24" s="25"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="25"/>
-      <c r="X24" s="25"/>
-      <c r="Y24" s="25" t="s">
+      <c r="AX24" s="22"/>
+      <c r="AY24" s="22"/>
+      <c r="AZ24" s="22"/>
+      <c r="BA24" s="22"/>
+      <c r="BB24" s="22"/>
+      <c r="BC24" s="22"/>
+      <c r="BD24" s="22"/>
+      <c r="BE24" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF24" s="22"/>
+      <c r="BG24" s="22"/>
+      <c r="BH24" s="22"/>
+      <c r="BI24" s="22"/>
+      <c r="BJ24" s="22"/>
+      <c r="BK24" s="22"/>
+      <c r="BL24" s="22"/>
+      <c r="BM24" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="Z24" s="25"/>
-      <c r="AA24" s="25"/>
-      <c r="AB24" s="25"/>
-      <c r="AC24" s="25"/>
-      <c r="AD24" s="25"/>
-      <c r="AE24" s="25"/>
-      <c r="AF24" s="25"/>
-      <c r="AG24" s="39">
-        <v>59</v>
-      </c>
-      <c r="AH24" s="39"/>
-      <c r="AI24" s="39"/>
-      <c r="AJ24" s="39"/>
-      <c r="AK24" s="39"/>
-      <c r="AL24" s="39"/>
-      <c r="AM24" s="39"/>
-      <c r="AN24" s="39"/>
-      <c r="AO24" s="39">
-        <v>96</v>
-      </c>
-      <c r="AP24" s="39"/>
-      <c r="AQ24" s="39"/>
-      <c r="AR24" s="39"/>
-      <c r="AS24" s="39"/>
-      <c r="AT24" s="39"/>
-      <c r="AU24" s="39"/>
-      <c r="AV24" s="39"/>
-      <c r="AW24" s="39">
-        <v>65</v>
-      </c>
-      <c r="AX24" s="39"/>
-      <c r="AY24" s="39"/>
-      <c r="AZ24" s="39"/>
-      <c r="BA24" s="39"/>
-      <c r="BB24" s="39"/>
-      <c r="BC24" s="39"/>
-      <c r="BD24" s="39"/>
-      <c r="BE24" s="39" t="s">
+      <c r="BN24" s="22"/>
+      <c r="BO24" s="22"/>
+      <c r="BP24" s="22"/>
+      <c r="BQ24" s="22"/>
+      <c r="BR24" s="22"/>
+      <c r="BS24" s="22"/>
+      <c r="BT24" s="22"/>
+      <c r="BU24" s="22">
         <v>69</v>
       </c>
-      <c r="BF24" s="39"/>
-      <c r="BG24" s="39"/>
-      <c r="BH24" s="39"/>
-      <c r="BI24" s="39"/>
-      <c r="BJ24" s="39"/>
-      <c r="BK24" s="39"/>
-      <c r="BL24" s="39"/>
-      <c r="BM24" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="BN24" s="39"/>
-      <c r="BO24" s="39"/>
-      <c r="BP24" s="39"/>
-      <c r="BQ24" s="39"/>
-      <c r="BR24" s="39"/>
-      <c r="BS24" s="39"/>
-      <c r="BT24" s="39"/>
-      <c r="BU24" s="39">
+      <c r="BV24" s="22"/>
+      <c r="BW24" s="22"/>
+      <c r="BX24" s="22"/>
+      <c r="BY24" s="22"/>
+      <c r="BZ24" s="22"/>
+      <c r="CA24" s="22"/>
+      <c r="CB24" s="22"/>
+      <c r="CC24" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="CD24" s="22"/>
+      <c r="CE24" s="22"/>
+      <c r="CF24" s="22"/>
+      <c r="CG24" s="22"/>
+      <c r="CH24" s="22"/>
+      <c r="CI24" s="22"/>
+      <c r="CJ24" s="22"/>
+      <c r="CK24" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="BV24" s="39"/>
-      <c r="BW24" s="39"/>
-      <c r="BX24" s="39"/>
-      <c r="BY24" s="39"/>
-      <c r="BZ24" s="39"/>
-      <c r="CA24" s="39"/>
-      <c r="CB24" s="39"/>
-      <c r="CC24" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="CD24" s="39"/>
-      <c r="CE24" s="39"/>
-      <c r="CF24" s="39"/>
-      <c r="CG24" s="39"/>
-      <c r="CH24" s="39"/>
-      <c r="CI24" s="39"/>
-      <c r="CJ24" s="39"/>
-      <c r="CK24" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="CL24" s="39"/>
-      <c r="CM24" s="39"/>
-      <c r="CN24" s="39"/>
-      <c r="CO24" s="39"/>
-      <c r="CP24" s="39"/>
-      <c r="CQ24" s="39"/>
-      <c r="CR24" s="39"/>
+      <c r="CL24" s="22"/>
+      <c r="CM24" s="22"/>
+      <c r="CN24" s="22"/>
+      <c r="CO24" s="22"/>
+      <c r="CP24" s="22"/>
+      <c r="CQ24" s="22"/>
+      <c r="CR24" s="22"/>
     </row>
     <row r="25" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
@@ -4121,180 +4160,180 @@
       </c>
     </row>
     <row r="26" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21" t="s">
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21" t="s">
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21" t="s">
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="R26" s="21"/>
-      <c r="S26" s="21"/>
-      <c r="T26" s="21" t="s">
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="U26" s="21"/>
-      <c r="V26" s="21"/>
-      <c r="W26" s="21"/>
-      <c r="X26" s="21"/>
-      <c r="Y26" s="21" t="s">
+      <c r="U26" s="23"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="23"/>
+      <c r="X26" s="23"/>
+      <c r="Y26" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="21"/>
-      <c r="AA26" s="21"/>
-      <c r="AB26" s="21"/>
-      <c r="AC26" s="21"/>
-      <c r="AD26" s="21" t="s">
+      <c r="Z26" s="23"/>
+      <c r="AA26" s="23"/>
+      <c r="AB26" s="23"/>
+      <c r="AC26" s="23"/>
+      <c r="AD26" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="AE26" s="21"/>
-      <c r="AF26" s="21"/>
-      <c r="AG26" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH26" s="23"/>
-      <c r="AI26" s="23"/>
-      <c r="AJ26" s="23"/>
-      <c r="AK26" s="23"/>
-      <c r="AL26" s="23"/>
-      <c r="AM26" s="23"/>
-      <c r="AN26" s="23"/>
-      <c r="AO26" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP26" s="23"/>
-      <c r="AQ26" s="23"/>
-      <c r="AR26" s="23"/>
-      <c r="AS26" s="23"/>
-      <c r="AT26" s="23"/>
-      <c r="AU26" s="23"/>
-      <c r="AV26" s="23"/>
-      <c r="AW26" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="AX26" s="23"/>
-      <c r="AY26" s="23"/>
-      <c r="AZ26" s="23"/>
-      <c r="BA26" s="23"/>
-      <c r="BB26" s="23"/>
-      <c r="BC26" s="23"/>
-      <c r="BD26" s="23"/>
-      <c r="BE26" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="BF26" s="23"/>
-      <c r="BG26" s="23"/>
-      <c r="BH26" s="23"/>
-      <c r="BI26" s="23"/>
-      <c r="BJ26" s="23"/>
-      <c r="BK26" s="23"/>
-      <c r="BL26" s="23"/>
-      <c r="BM26" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="BN26" s="23"/>
-      <c r="BO26" s="23"/>
-      <c r="BP26" s="23"/>
-      <c r="BQ26" s="23"/>
-      <c r="BR26" s="23"/>
-      <c r="BS26" s="23"/>
-      <c r="BT26" s="23"/>
-      <c r="BU26" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="BV26" s="23"/>
-      <c r="BW26" s="23"/>
-      <c r="BX26" s="23"/>
-      <c r="BY26" s="23"/>
-      <c r="BZ26" s="23"/>
-      <c r="CA26" s="23"/>
-      <c r="CB26" s="23"/>
-      <c r="CC26" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="CD26" s="23"/>
-      <c r="CE26" s="23"/>
-      <c r="CF26" s="23"/>
-      <c r="CG26" s="23"/>
-      <c r="CH26" s="23"/>
-      <c r="CI26" s="23"/>
-      <c r="CJ26" s="23"/>
-      <c r="CK26" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="CL26" s="23"/>
-      <c r="CM26" s="23"/>
-      <c r="CN26" s="23"/>
-      <c r="CO26" s="23"/>
-      <c r="CP26" s="23"/>
-      <c r="CQ26" s="23"/>
-      <c r="CR26" s="23"/>
+      <c r="AE26" s="23"/>
+      <c r="AF26" s="23"/>
+      <c r="AG26" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH26" s="21"/>
+      <c r="AI26" s="21"/>
+      <c r="AJ26" s="21"/>
+      <c r="AK26" s="21"/>
+      <c r="AL26" s="21"/>
+      <c r="AM26" s="21"/>
+      <c r="AN26" s="21"/>
+      <c r="AO26" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP26" s="21"/>
+      <c r="AQ26" s="21"/>
+      <c r="AR26" s="21"/>
+      <c r="AS26" s="21"/>
+      <c r="AT26" s="21"/>
+      <c r="AU26" s="21"/>
+      <c r="AV26" s="21"/>
+      <c r="AW26" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX26" s="21"/>
+      <c r="AY26" s="21"/>
+      <c r="AZ26" s="21"/>
+      <c r="BA26" s="21"/>
+      <c r="BB26" s="21"/>
+      <c r="BC26" s="21"/>
+      <c r="BD26" s="21"/>
+      <c r="BE26" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="BF26" s="21"/>
+      <c r="BG26" s="21"/>
+      <c r="BH26" s="21"/>
+      <c r="BI26" s="21"/>
+      <c r="BJ26" s="21"/>
+      <c r="BK26" s="21"/>
+      <c r="BL26" s="21"/>
+      <c r="BM26" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="BN26" s="21"/>
+      <c r="BO26" s="21"/>
+      <c r="BP26" s="21"/>
+      <c r="BQ26" s="21"/>
+      <c r="BR26" s="21"/>
+      <c r="BS26" s="21"/>
+      <c r="BT26" s="21"/>
+      <c r="BU26" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="BV26" s="21"/>
+      <c r="BW26" s="21"/>
+      <c r="BX26" s="21"/>
+      <c r="BY26" s="21"/>
+      <c r="BZ26" s="21"/>
+      <c r="CA26" s="21"/>
+      <c r="CB26" s="21"/>
+      <c r="CC26" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="CD26" s="21"/>
+      <c r="CE26" s="21"/>
+      <c r="CF26" s="21"/>
+      <c r="CG26" s="21"/>
+      <c r="CH26" s="21"/>
+      <c r="CI26" s="21"/>
+      <c r="CJ26" s="21"/>
+      <c r="CK26" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="CL26" s="21"/>
+      <c r="CM26" s="21"/>
+      <c r="CN26" s="21"/>
+      <c r="CO26" s="21"/>
+      <c r="CP26" s="21"/>
+      <c r="CQ26" s="21"/>
+      <c r="CR26" s="21"/>
     </row>
     <row r="27" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A27" s="21">
+      <c r="A27" s="23">
         <v>10</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21">
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23">
         <v>8</v>
       </c>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21">
-        <v>0</v>
-      </c>
-      <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
-      <c r="Q27" s="21">
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23">
+        <v>0</v>
+      </c>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23">
         <v>3</v>
       </c>
-      <c r="R27" s="21"/>
-      <c r="S27" s="21"/>
-      <c r="T27" s="21">
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23">
         <v>19</v>
       </c>
-      <c r="U27" s="21"/>
-      <c r="V27" s="21"/>
-      <c r="W27" s="21"/>
-      <c r="X27" s="21"/>
-      <c r="Y27" s="21">
+      <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="23">
         <v>21</v>
       </c>
-      <c r="Z27" s="21"/>
-      <c r="AA27" s="21"/>
-      <c r="AB27" s="21"/>
-      <c r="AC27" s="21"/>
-      <c r="AD27" s="21">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="21"/>
-      <c r="AF27" s="21"/>
+      <c r="Z27" s="23"/>
+      <c r="AA27" s="23"/>
+      <c r="AB27" s="23"/>
+      <c r="AC27" s="23"/>
+      <c r="AD27" s="23">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="23"/>
+      <c r="AF27" s="23"/>
       <c r="AG27">
         <f>AN25</f>
         <v>1</v>
@@ -4553,267 +4592,267 @@
       </c>
     </row>
     <row r="28" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21" t="s">
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="O28" s="21"/>
-      <c r="P28" s="21"/>
-      <c r="Q28" s="21" t="s">
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+      <c r="Y28" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="R28" s="21"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="21" t="s">
+      <c r="Z28" s="23"/>
+      <c r="AA28" s="23"/>
+      <c r="AB28" s="23"/>
+      <c r="AC28" s="23"/>
+      <c r="AD28" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="U28" s="21"/>
-      <c r="V28" s="21"/>
-      <c r="W28" s="21"/>
-      <c r="X28" s="21"/>
-      <c r="Y28" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z28" s="21"/>
-      <c r="AA28" s="21"/>
-      <c r="AB28" s="21"/>
-      <c r="AC28" s="21"/>
-      <c r="AD28" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE28" s="21"/>
-      <c r="AF28" s="21"/>
-      <c r="AG28" s="23" t="s">
+      <c r="AE28" s="23"/>
+      <c r="AF28" s="23"/>
+      <c r="AG28" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH28" s="21"/>
+      <c r="AI28" s="21"/>
+      <c r="AJ28" s="21"/>
+      <c r="AK28" s="21"/>
+      <c r="AL28" s="21"/>
+      <c r="AM28" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN28" s="21"/>
+      <c r="AO28" s="21"/>
+      <c r="AP28" s="21"/>
+      <c r="AQ28" s="21"/>
+      <c r="AR28" s="21"/>
+      <c r="AS28" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AH28" s="23"/>
-      <c r="AI28" s="23"/>
-      <c r="AJ28" s="23"/>
-      <c r="AK28" s="23"/>
-      <c r="AL28" s="23"/>
-      <c r="AM28" s="23" t="s">
+      <c r="AT28" s="21"/>
+      <c r="AU28" s="21"/>
+      <c r="AV28" s="21"/>
+      <c r="AW28" s="21"/>
+      <c r="AX28" s="21"/>
+      <c r="AY28" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="AN28" s="23"/>
-      <c r="AO28" s="23"/>
-      <c r="AP28" s="23"/>
-      <c r="AQ28" s="23"/>
-      <c r="AR28" s="23"/>
-      <c r="AS28" s="23" t="s">
+      <c r="AZ28" s="21"/>
+      <c r="BA28" s="21"/>
+      <c r="BB28" s="21"/>
+      <c r="BC28" s="21"/>
+      <c r="BD28" s="21"/>
+      <c r="BE28" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="AT28" s="23"/>
-      <c r="AU28" s="23"/>
-      <c r="AV28" s="23"/>
-      <c r="AW28" s="23"/>
-      <c r="AX28" s="23"/>
-      <c r="AY28" s="23" t="s">
+      <c r="BF28" s="21"/>
+      <c r="BG28" s="21"/>
+      <c r="BH28" s="21"/>
+      <c r="BI28" s="21"/>
+      <c r="BJ28" s="21"/>
+      <c r="BK28" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="AZ28" s="23"/>
-      <c r="BA28" s="23"/>
-      <c r="BB28" s="23"/>
-      <c r="BC28" s="23"/>
-      <c r="BD28" s="23"/>
-      <c r="BE28" s="23" t="s">
+      <c r="BL28" s="21"/>
+      <c r="BM28" s="21"/>
+      <c r="BN28" s="21"/>
+      <c r="BO28" s="21"/>
+      <c r="BP28" s="21"/>
+      <c r="BQ28" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="BF28" s="23"/>
-      <c r="BG28" s="23"/>
-      <c r="BH28" s="23"/>
-      <c r="BI28" s="23"/>
-      <c r="BJ28" s="23"/>
-      <c r="BK28" s="23" t="s">
+      <c r="BR28" s="21"/>
+      <c r="BS28" s="21"/>
+      <c r="BT28" s="21"/>
+      <c r="BU28" s="21"/>
+      <c r="BV28" s="21"/>
+      <c r="BW28" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="BL28" s="23"/>
-      <c r="BM28" s="23"/>
-      <c r="BN28" s="23"/>
-      <c r="BO28" s="23"/>
-      <c r="BP28" s="23"/>
-      <c r="BQ28" s="23" t="s">
+      <c r="BX28" s="21"/>
+      <c r="BY28" s="21"/>
+      <c r="BZ28" s="21"/>
+      <c r="CA28" s="21"/>
+      <c r="CB28" s="21"/>
+      <c r="CC28" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="BR28" s="23"/>
-      <c r="BS28" s="23"/>
-      <c r="BT28" s="23"/>
-      <c r="BU28" s="23"/>
-      <c r="BV28" s="23"/>
-      <c r="BW28" s="23" t="s">
+      <c r="CD28" s="21"/>
+      <c r="CE28" s="21"/>
+      <c r="CF28" s="21"/>
+      <c r="CG28" s="21"/>
+      <c r="CH28" s="21"/>
+      <c r="CI28" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="BX28" s="23"/>
-      <c r="BY28" s="23"/>
-      <c r="BZ28" s="23"/>
-      <c r="CA28" s="23"/>
-      <c r="CB28" s="23"/>
-      <c r="CC28" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="CD28" s="23"/>
-      <c r="CE28" s="23"/>
-      <c r="CF28" s="23"/>
-      <c r="CG28" s="23"/>
-      <c r="CH28" s="23"/>
-      <c r="CI28" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="CJ28" s="23"/>
-      <c r="CK28" s="23"/>
-      <c r="CL28" s="23"/>
-      <c r="CM28" s="23"/>
-      <c r="CN28" s="23"/>
+      <c r="CJ28" s="21"/>
+      <c r="CK28" s="21"/>
+      <c r="CL28" s="21"/>
+      <c r="CM28" s="21"/>
+      <c r="CN28" s="21"/>
     </row>
     <row r="29" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="A29" s="21">
+      <c r="A29" s="23">
         <f>A27</f>
         <v>10</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="22">
-        <f>100/(2^5-1)*I27</f>
-        <v>25.806451612903224</v>
-      </c>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="23" t="str">
-        <f>LOOKUP(N27,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$18)</f>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="24">
+        <f>'Data package'!$B$21*I27+'Data package'!$B$18</f>
+        <v>3.3870967741935485</v>
+      </c>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="21" t="str">
+        <f ca="1">LOOKUP(N27,'Data package'!$D$11:$D$18,'Data package'!$E$11:$E$21)</f>
         <v>no error</v>
       </c>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="24">
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="25">
         <f>100/(2^3-1)*Q27</f>
         <v>42.857142857142861</v>
       </c>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="24">
-        <f>'Data package'!$B$27*T27+'Data package'!$B$24</f>
+      <c r="R29" s="25"/>
+      <c r="S29" s="25"/>
+      <c r="T29" s="25">
+        <f>'Data package'!$B$30*T27+'Data package'!$B$27</f>
         <v>22.903225806451616</v>
       </c>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23"/>
-      <c r="Y29" s="23">
+      <c r="U29" s="21"/>
+      <c r="V29" s="21"/>
+      <c r="W29" s="21"/>
+      <c r="X29" s="21"/>
+      <c r="Y29" s="21">
         <f>Y27</f>
         <v>21</v>
       </c>
-      <c r="Z29" s="23"/>
-      <c r="AA29" s="23"/>
-      <c r="AB29" s="23"/>
-      <c r="AC29" s="23"/>
-      <c r="AD29" s="23">
-        <f>LOOKUP(AD27,'Data package'!$A$64:$A$68,'Data package'!$B$64:$B$68)</f>
-        <v>1</v>
-      </c>
-      <c r="AE29" s="23"/>
-      <c r="AF29" s="23"/>
-      <c r="AG29" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH29" s="23"/>
-      <c r="AI29" s="23"/>
-      <c r="AJ29" s="23"/>
-      <c r="AK29" s="23"/>
-      <c r="AL29" s="23"/>
-      <c r="AM29" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="AN29" s="23"/>
-      <c r="AO29" s="23"/>
-      <c r="AP29" s="23"/>
-      <c r="AQ29" s="23"/>
-      <c r="AR29" s="23"/>
-      <c r="AS29" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="AT29" s="23"/>
-      <c r="AU29" s="23"/>
-      <c r="AV29" s="23"/>
-      <c r="AW29" s="23"/>
-      <c r="AX29" s="23"/>
-      <c r="AY29" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="AZ29" s="23"/>
-      <c r="BA29" s="23"/>
-      <c r="BB29" s="23"/>
-      <c r="BC29" s="23"/>
-      <c r="BD29" s="23"/>
-      <c r="BE29" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="BF29" s="23"/>
-      <c r="BG29" s="23"/>
-      <c r="BH29" s="23"/>
-      <c r="BI29" s="23"/>
-      <c r="BJ29" s="23"/>
-      <c r="BK29" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="BL29" s="23"/>
-      <c r="BM29" s="23"/>
-      <c r="BN29" s="23"/>
-      <c r="BO29" s="23"/>
-      <c r="BP29" s="23"/>
-      <c r="BQ29" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="BR29" s="23"/>
-      <c r="BS29" s="23"/>
-      <c r="BT29" s="23"/>
-      <c r="BU29" s="23"/>
-      <c r="BV29" s="23"/>
-      <c r="BW29" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="BX29" s="23"/>
-      <c r="BY29" s="23"/>
-      <c r="BZ29" s="23"/>
-      <c r="CA29" s="23"/>
-      <c r="CB29" s="23"/>
-      <c r="CC29" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="CD29" s="23"/>
-      <c r="CE29" s="23"/>
-      <c r="CF29" s="23"/>
-      <c r="CG29" s="23"/>
-      <c r="CH29" s="23"/>
-      <c r="CI29" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="CJ29" s="23"/>
-      <c r="CK29" s="23"/>
-      <c r="CL29" s="23"/>
-      <c r="CM29" s="23"/>
-      <c r="CN29" s="23"/>
+      <c r="Z29" s="21"/>
+      <c r="AA29" s="21"/>
+      <c r="AB29" s="21"/>
+      <c r="AC29" s="21"/>
+      <c r="AD29" s="21">
+        <f>LOOKUP(AD27,'Data package'!$A$67:$A$71,'Data package'!$B$67:$B$71)</f>
+        <v>1</v>
+      </c>
+      <c r="AE29" s="21"/>
+      <c r="AF29" s="21"/>
+      <c r="AG29" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH29" s="21"/>
+      <c r="AI29" s="21"/>
+      <c r="AJ29" s="21"/>
+      <c r="AK29" s="21"/>
+      <c r="AL29" s="21"/>
+      <c r="AM29" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN29" s="21"/>
+      <c r="AO29" s="21"/>
+      <c r="AP29" s="21"/>
+      <c r="AQ29" s="21"/>
+      <c r="AR29" s="21"/>
+      <c r="AS29" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT29" s="21"/>
+      <c r="AU29" s="21"/>
+      <c r="AV29" s="21"/>
+      <c r="AW29" s="21"/>
+      <c r="AX29" s="21"/>
+      <c r="AY29" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ29" s="21"/>
+      <c r="BA29" s="21"/>
+      <c r="BB29" s="21"/>
+      <c r="BC29" s="21"/>
+      <c r="BD29" s="21"/>
+      <c r="BE29" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="BF29" s="21"/>
+      <c r="BG29" s="21"/>
+      <c r="BH29" s="21"/>
+      <c r="BI29" s="21"/>
+      <c r="BJ29" s="21"/>
+      <c r="BK29" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="BL29" s="21"/>
+      <c r="BM29" s="21"/>
+      <c r="BN29" s="21"/>
+      <c r="BO29" s="21"/>
+      <c r="BP29" s="21"/>
+      <c r="BQ29" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="BR29" s="21"/>
+      <c r="BS29" s="21"/>
+      <c r="BT29" s="21"/>
+      <c r="BU29" s="21"/>
+      <c r="BV29" s="21"/>
+      <c r="BW29" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="BX29" s="21"/>
+      <c r="BY29" s="21"/>
+      <c r="BZ29" s="21"/>
+      <c r="CA29" s="21"/>
+      <c r="CB29" s="21"/>
+      <c r="CC29" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="CD29" s="21"/>
+      <c r="CE29" s="21"/>
+      <c r="CF29" s="21"/>
+      <c r="CG29" s="21"/>
+      <c r="CH29" s="21"/>
+      <c r="CI29" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="CJ29" s="21"/>
+      <c r="CK29" s="21"/>
+      <c r="CL29" s="21"/>
+      <c r="CM29" s="21"/>
+      <c r="CN29" s="21"/>
     </row>
     <row r="30" spans="1:96" x14ac:dyDescent="0.3">
       <c r="AG30">
@@ -5058,255 +5097,229 @@
       </c>
     </row>
     <row r="31" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG31" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH31" s="23"/>
-      <c r="AI31" s="23"/>
-      <c r="AJ31" s="23"/>
-      <c r="AK31" s="23"/>
-      <c r="AL31" s="23"/>
-      <c r="AM31" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN31" s="23"/>
-      <c r="AO31" s="23"/>
-      <c r="AP31" s="23"/>
-      <c r="AQ31" s="23"/>
-      <c r="AR31" s="23"/>
-      <c r="AS31" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="AT31" s="23"/>
-      <c r="AU31" s="23"/>
-      <c r="AV31" s="23"/>
-      <c r="AW31" s="23"/>
-      <c r="AX31" s="23"/>
-      <c r="AY31" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="AZ31" s="23"/>
-      <c r="BA31" s="23"/>
-      <c r="BB31" s="23"/>
-      <c r="BC31" s="23"/>
-      <c r="BD31" s="23"/>
-      <c r="BE31" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="BF31" s="23"/>
-      <c r="BG31" s="23"/>
-      <c r="BH31" s="23"/>
-      <c r="BI31" s="23"/>
-      <c r="BJ31" s="23"/>
-      <c r="BK31" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="BL31" s="23"/>
-      <c r="BM31" s="23"/>
-      <c r="BN31" s="23"/>
-      <c r="BO31" s="23"/>
-      <c r="BP31" s="23"/>
-      <c r="BQ31" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="BR31" s="23"/>
-      <c r="BS31" s="23"/>
-      <c r="BT31" s="23"/>
-      <c r="BU31" s="23"/>
-      <c r="BV31" s="23"/>
-      <c r="BW31" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="BX31" s="23"/>
-      <c r="BY31" s="23"/>
-      <c r="BZ31" s="23"/>
-      <c r="CA31" s="23"/>
-      <c r="CB31" s="23"/>
-      <c r="CC31" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="CD31" s="23"/>
-      <c r="CE31" s="23"/>
-      <c r="CF31" s="23"/>
-      <c r="CG31" s="23"/>
-      <c r="CH31" s="23"/>
-      <c r="CI31" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="CJ31" s="23"/>
-      <c r="CK31" s="23"/>
-      <c r="CL31" s="23"/>
-      <c r="CM31" s="23"/>
-      <c r="CN31" s="23"/>
+      <c r="AG31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH31" s="21"/>
+      <c r="AI31" s="21"/>
+      <c r="AJ31" s="21"/>
+      <c r="AK31" s="21"/>
+      <c r="AL31" s="21"/>
+      <c r="AM31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN31" s="21"/>
+      <c r="AO31" s="21"/>
+      <c r="AP31" s="21"/>
+      <c r="AQ31" s="21"/>
+      <c r="AR31" s="21"/>
+      <c r="AS31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT31" s="21"/>
+      <c r="AU31" s="21"/>
+      <c r="AV31" s="21"/>
+      <c r="AW31" s="21"/>
+      <c r="AX31" s="21"/>
+      <c r="AY31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="AZ31" s="21"/>
+      <c r="BA31" s="21"/>
+      <c r="BB31" s="21"/>
+      <c r="BC31" s="21"/>
+      <c r="BD31" s="21"/>
+      <c r="BE31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="BF31" s="21"/>
+      <c r="BG31" s="21"/>
+      <c r="BH31" s="21"/>
+      <c r="BI31" s="21"/>
+      <c r="BJ31" s="21"/>
+      <c r="BK31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="BL31" s="21"/>
+      <c r="BM31" s="21"/>
+      <c r="BN31" s="21"/>
+      <c r="BO31" s="21"/>
+      <c r="BP31" s="21"/>
+      <c r="BQ31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="BR31" s="21"/>
+      <c r="BS31" s="21"/>
+      <c r="BT31" s="21"/>
+      <c r="BU31" s="21"/>
+      <c r="BV31" s="21"/>
+      <c r="BW31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="BX31" s="21"/>
+      <c r="BY31" s="21"/>
+      <c r="BZ31" s="21"/>
+      <c r="CA31" s="21"/>
+      <c r="CB31" s="21"/>
+      <c r="CC31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="CD31" s="21"/>
+      <c r="CE31" s="21"/>
+      <c r="CF31" s="21"/>
+      <c r="CG31" s="21"/>
+      <c r="CH31" s="21"/>
+      <c r="CI31" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="CJ31" s="21"/>
+      <c r="CK31" s="21"/>
+      <c r="CL31" s="21"/>
+      <c r="CM31" s="21"/>
+      <c r="CN31" s="21"/>
     </row>
     <row r="32" spans="1:96" x14ac:dyDescent="0.3">
-      <c r="AG32" s="23">
+      <c r="AG32" s="21">
         <v>25</v>
       </c>
-      <c r="AH32" s="23"/>
-      <c r="AI32" s="23"/>
-      <c r="AJ32" s="23"/>
-      <c r="AK32" s="23"/>
-      <c r="AL32" s="23"/>
-      <c r="AM32" s="23">
+      <c r="AH32" s="21"/>
+      <c r="AI32" s="21"/>
+      <c r="AJ32" s="21"/>
+      <c r="AK32" s="21"/>
+      <c r="AL32" s="21"/>
+      <c r="AM32" s="21">
         <v>25</v>
       </c>
-      <c r="AN32" s="23"/>
-      <c r="AO32" s="23"/>
-      <c r="AP32" s="23"/>
-      <c r="AQ32" s="23"/>
-      <c r="AR32" s="23"/>
-      <c r="AS32" s="23">
+      <c r="AN32" s="21"/>
+      <c r="AO32" s="21"/>
+      <c r="AP32" s="21"/>
+      <c r="AQ32" s="21"/>
+      <c r="AR32" s="21"/>
+      <c r="AS32" s="21">
         <v>25</v>
       </c>
-      <c r="AT32" s="23"/>
-      <c r="AU32" s="23"/>
-      <c r="AV32" s="23"/>
-      <c r="AW32" s="23"/>
-      <c r="AX32" s="23"/>
-      <c r="AY32" s="23">
+      <c r="AT32" s="21"/>
+      <c r="AU32" s="21"/>
+      <c r="AV32" s="21"/>
+      <c r="AW32" s="21"/>
+      <c r="AX32" s="21"/>
+      <c r="AY32" s="21">
         <v>25</v>
       </c>
-      <c r="AZ32" s="23"/>
-      <c r="BA32" s="23"/>
-      <c r="BB32" s="23"/>
-      <c r="BC32" s="23"/>
-      <c r="BD32" s="23"/>
-      <c r="BE32" s="23">
+      <c r="AZ32" s="21"/>
+      <c r="BA32" s="21"/>
+      <c r="BB32" s="21"/>
+      <c r="BC32" s="21"/>
+      <c r="BD32" s="21"/>
+      <c r="BE32" s="21">
         <v>26</v>
       </c>
-      <c r="BF32" s="23"/>
-      <c r="BG32" s="23"/>
-      <c r="BH32" s="23"/>
-      <c r="BI32" s="23"/>
-      <c r="BJ32" s="23"/>
-      <c r="BK32" s="23">
+      <c r="BF32" s="21"/>
+      <c r="BG32" s="21"/>
+      <c r="BH32" s="21"/>
+      <c r="BI32" s="21"/>
+      <c r="BJ32" s="21"/>
+      <c r="BK32" s="21">
         <v>26</v>
       </c>
-      <c r="BL32" s="23"/>
-      <c r="BM32" s="23"/>
-      <c r="BN32" s="23"/>
-      <c r="BO32" s="23"/>
-      <c r="BP32" s="23"/>
-      <c r="BQ32" s="23">
+      <c r="BL32" s="21"/>
+      <c r="BM32" s="21"/>
+      <c r="BN32" s="21"/>
+      <c r="BO32" s="21"/>
+      <c r="BP32" s="21"/>
+      <c r="BQ32" s="21">
         <v>26</v>
       </c>
-      <c r="BR32" s="23"/>
-      <c r="BS32" s="23"/>
-      <c r="BT32" s="23"/>
-      <c r="BU32" s="23"/>
-      <c r="BV32" s="23"/>
-      <c r="BW32" s="23">
+      <c r="BR32" s="21"/>
+      <c r="BS32" s="21"/>
+      <c r="BT32" s="21"/>
+      <c r="BU32" s="21"/>
+      <c r="BV32" s="21"/>
+      <c r="BW32" s="21">
         <v>26</v>
       </c>
-      <c r="BX32" s="23"/>
-      <c r="BY32" s="23"/>
-      <c r="BZ32" s="23"/>
-      <c r="CA32" s="23"/>
-      <c r="CB32" s="23"/>
-      <c r="CC32" s="23">
+      <c r="BX32" s="21"/>
+      <c r="BY32" s="21"/>
+      <c r="BZ32" s="21"/>
+      <c r="CA32" s="21"/>
+      <c r="CB32" s="21"/>
+      <c r="CC32" s="21">
         <v>26</v>
       </c>
-      <c r="CD32" s="23"/>
-      <c r="CE32" s="23"/>
-      <c r="CF32" s="23"/>
-      <c r="CG32" s="23"/>
-      <c r="CH32" s="23"/>
-      <c r="CI32" s="23">
+      <c r="CD32" s="21"/>
+      <c r="CE32" s="21"/>
+      <c r="CF32" s="21"/>
+      <c r="CG32" s="21"/>
+      <c r="CH32" s="21"/>
+      <c r="CI32" s="21">
         <v>26</v>
       </c>
-      <c r="CJ32" s="23"/>
-      <c r="CK32" s="23"/>
-      <c r="CL32" s="23"/>
-      <c r="CM32" s="23"/>
-      <c r="CN32" s="23"/>
+      <c r="CJ32" s="21"/>
+      <c r="CK32" s="21"/>
+      <c r="CL32" s="21"/>
+      <c r="CM32" s="21"/>
+      <c r="CN32" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="166">
-    <mergeCell ref="BK32:BP32"/>
-    <mergeCell ref="BQ32:BV32"/>
-    <mergeCell ref="BW32:CB32"/>
-    <mergeCell ref="CC32:CH32"/>
-    <mergeCell ref="CI32:CN32"/>
-    <mergeCell ref="AG32:AL32"/>
-    <mergeCell ref="AM32:AR32"/>
-    <mergeCell ref="AS32:AX32"/>
-    <mergeCell ref="AY32:BD32"/>
-    <mergeCell ref="BE32:BJ32"/>
-    <mergeCell ref="BK31:BP31"/>
-    <mergeCell ref="BQ31:BV31"/>
-    <mergeCell ref="BW31:CB31"/>
-    <mergeCell ref="CC31:CH31"/>
-    <mergeCell ref="CI31:CN31"/>
-    <mergeCell ref="AG31:AL31"/>
-    <mergeCell ref="AM31:AR31"/>
-    <mergeCell ref="AS31:AX31"/>
-    <mergeCell ref="AY31:BD31"/>
-    <mergeCell ref="BE31:BJ31"/>
-    <mergeCell ref="BK29:BP29"/>
-    <mergeCell ref="BQ29:BV29"/>
-    <mergeCell ref="BW29:CB29"/>
-    <mergeCell ref="CC29:CH29"/>
-    <mergeCell ref="CI29:CN29"/>
-    <mergeCell ref="AG29:AL29"/>
-    <mergeCell ref="AM29:AR29"/>
-    <mergeCell ref="AS29:AX29"/>
-    <mergeCell ref="AY29:BD29"/>
-    <mergeCell ref="BE29:BJ29"/>
-    <mergeCell ref="BK28:BP28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="BW28:CB28"/>
-    <mergeCell ref="CC28:CH28"/>
-    <mergeCell ref="CI28:CN28"/>
-    <mergeCell ref="AG28:AL28"/>
-    <mergeCell ref="AM28:AR28"/>
-    <mergeCell ref="AS28:AX28"/>
-    <mergeCell ref="AY28:BD28"/>
-    <mergeCell ref="BE28:BJ28"/>
-    <mergeCell ref="BU24:CB24"/>
-    <mergeCell ref="CC24:CJ24"/>
-    <mergeCell ref="CK24:CR24"/>
-    <mergeCell ref="AG26:AN26"/>
-    <mergeCell ref="AO26:AV26"/>
-    <mergeCell ref="AW26:BD26"/>
-    <mergeCell ref="BE26:BL26"/>
-    <mergeCell ref="BM26:BT26"/>
-    <mergeCell ref="BU26:CB26"/>
-    <mergeCell ref="CC26:CJ26"/>
-    <mergeCell ref="CK26:CR26"/>
-    <mergeCell ref="AG24:AN24"/>
-    <mergeCell ref="AO24:AV24"/>
-    <mergeCell ref="AW24:BD24"/>
-    <mergeCell ref="BE24:BL24"/>
-    <mergeCell ref="BM24:BT24"/>
-    <mergeCell ref="Y28:AC28"/>
-    <mergeCell ref="AD28:AF28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="Q29:S29"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Y29:AC29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="Q28:S28"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="Y26:AC26"/>
-    <mergeCell ref="AD26:AF26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="Q27:S27"/>
-    <mergeCell ref="T27:X27"/>
-    <mergeCell ref="Y27:AC27"/>
-    <mergeCell ref="AD27:AF27"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="I26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AD19:AF19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:S20"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="Y20:AC20"/>
+    <mergeCell ref="AD20:AF20"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I19:M19"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="Q19:S19"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="Q15:X15"/>
+    <mergeCell ref="Y15:AF15"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:M18"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AF18"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Q10:S10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="AD11:AF11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="Q6:X6"/>
+    <mergeCell ref="Y6:AF6"/>
+    <mergeCell ref="AD9:AF9"/>
+    <mergeCell ref="AD8:AF8"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="T9:X9"/>
     <mergeCell ref="A23:AF23"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="I24:P24"/>
@@ -5331,64 +5344,90 @@
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="Y6:AF6"/>
-    <mergeCell ref="AD9:AF9"/>
-    <mergeCell ref="AD8:AF8"/>
-    <mergeCell ref="Y9:AC9"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="T9:X9"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="Y10:AC10"/>
-    <mergeCell ref="T10:X10"/>
-    <mergeCell ref="Q10:S10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="AD11:AF11"/>
-    <mergeCell ref="Y11:AC11"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="I15:P15"/>
-    <mergeCell ref="Q15:X15"/>
-    <mergeCell ref="Y15:AF15"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="Y17:AC17"/>
-    <mergeCell ref="AD17:AF17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="I18:M18"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="Q18:S18"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="Y18:AC18"/>
-    <mergeCell ref="AD18:AF18"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:S17"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="Y19:AC19"/>
-    <mergeCell ref="AD19:AF19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="I20:M20"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:S20"/>
-    <mergeCell ref="T20:X20"/>
-    <mergeCell ref="Y20:AC20"/>
-    <mergeCell ref="AD20:AF20"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="I19:M19"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="Q19:S19"/>
-    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="Y26:AC26"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="Q27:S27"/>
+    <mergeCell ref="T27:X27"/>
+    <mergeCell ref="Y27:AC27"/>
+    <mergeCell ref="AD27:AF27"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y28:AC28"/>
+    <mergeCell ref="AD28:AF28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AF29"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="BU24:CB24"/>
+    <mergeCell ref="CC24:CJ24"/>
+    <mergeCell ref="CK24:CR24"/>
+    <mergeCell ref="AG26:AN26"/>
+    <mergeCell ref="AO26:AV26"/>
+    <mergeCell ref="AW26:BD26"/>
+    <mergeCell ref="BE26:BL26"/>
+    <mergeCell ref="BM26:BT26"/>
+    <mergeCell ref="BU26:CB26"/>
+    <mergeCell ref="CC26:CJ26"/>
+    <mergeCell ref="CK26:CR26"/>
+    <mergeCell ref="AG24:AN24"/>
+    <mergeCell ref="AO24:AV24"/>
+    <mergeCell ref="AW24:BD24"/>
+    <mergeCell ref="BE24:BL24"/>
+    <mergeCell ref="BM24:BT24"/>
+    <mergeCell ref="BK28:BP28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="BW28:CB28"/>
+    <mergeCell ref="CC28:CH28"/>
+    <mergeCell ref="CI28:CN28"/>
+    <mergeCell ref="AG28:AL28"/>
+    <mergeCell ref="AM28:AR28"/>
+    <mergeCell ref="AS28:AX28"/>
+    <mergeCell ref="AY28:BD28"/>
+    <mergeCell ref="BE28:BJ28"/>
+    <mergeCell ref="BK29:BP29"/>
+    <mergeCell ref="BQ29:BV29"/>
+    <mergeCell ref="BW29:CB29"/>
+    <mergeCell ref="CC29:CH29"/>
+    <mergeCell ref="CI29:CN29"/>
+    <mergeCell ref="AG29:AL29"/>
+    <mergeCell ref="AM29:AR29"/>
+    <mergeCell ref="AS29:AX29"/>
+    <mergeCell ref="AY29:BD29"/>
+    <mergeCell ref="BE29:BJ29"/>
+    <mergeCell ref="BK31:BP31"/>
+    <mergeCell ref="BQ31:BV31"/>
+    <mergeCell ref="BW31:CB31"/>
+    <mergeCell ref="CC31:CH31"/>
+    <mergeCell ref="CI31:CN31"/>
+    <mergeCell ref="AG31:AL31"/>
+    <mergeCell ref="AM31:AR31"/>
+    <mergeCell ref="AS31:AX31"/>
+    <mergeCell ref="AY31:BD31"/>
+    <mergeCell ref="BE31:BJ31"/>
+    <mergeCell ref="BK32:BP32"/>
+    <mergeCell ref="BQ32:BV32"/>
+    <mergeCell ref="BW32:CB32"/>
+    <mergeCell ref="CC32:CH32"/>
+    <mergeCell ref="CI32:CN32"/>
+    <mergeCell ref="AG32:AL32"/>
+    <mergeCell ref="AM32:AR32"/>
+    <mergeCell ref="AS32:AX32"/>
+    <mergeCell ref="AY32:BD32"/>
+    <mergeCell ref="BE32:BJ32"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5417,44 +5456,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="11">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="K3" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="K3" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="12">
         <v>0.01</v>
       </c>
@@ -5473,8 +5512,8 @@
       <c r="I4" s="12">
         <v>10</v>
       </c>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
       <c r="M4" s="12">
         <v>0.01</v>
       </c>
@@ -5495,8 +5534,8 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="37" t="s">
-        <v>42</v>
+      <c r="B5" s="38" t="s">
+        <v>41</v>
       </c>
       <c r="C5" s="12">
         <v>0.01</v>
@@ -5525,8 +5564,8 @@
         <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="K5" s="37" t="s">
-        <v>42</v>
+      <c r="K5" s="38" t="s">
+        <v>41</v>
       </c>
       <c r="L5" s="12">
         <v>0.01</v>
@@ -5557,7 +5596,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="12">
         <v>0.02</v>
       </c>
@@ -5585,7 +5624,7 @@
         <f t="shared" si="2"/>
         <v>2E-3</v>
       </c>
-      <c r="K6" s="37"/>
+      <c r="K6" s="38"/>
       <c r="L6" s="12">
         <v>0.02</v>
       </c>
@@ -5615,7 +5654,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="37"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="12">
         <v>0.03</v>
       </c>
@@ -5643,7 +5682,7 @@
         <f t="shared" si="2"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K7" s="37"/>
+      <c r="K7" s="38"/>
       <c r="L7" s="12">
         <v>0.03</v>
       </c>
@@ -5673,7 +5712,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="37"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="12">
         <v>0.05</v>
       </c>
@@ -5701,7 +5740,7 @@
         <f t="shared" si="2"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K8" s="37"/>
+      <c r="K8" s="38"/>
       <c r="L8" s="12">
         <v>0.05</v>
       </c>
@@ -5731,7 +5770,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="37"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="12">
         <v>0.1</v>
       </c>
@@ -5759,7 +5798,7 @@
         <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
-      <c r="K9" s="37"/>
+      <c r="K9" s="38"/>
       <c r="L9" s="12">
         <v>0.1</v>
       </c>
@@ -5789,7 +5828,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="37"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="12">
         <v>0.2</v>
       </c>
@@ -5817,7 +5856,7 @@
         <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
-      <c r="K10" s="37"/>
+      <c r="K10" s="38"/>
       <c r="L10" s="12">
         <v>0.2</v>
       </c>
@@ -5847,7 +5886,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="37"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="12">
         <v>0.3</v>
       </c>
@@ -5875,7 +5914,7 @@
         <f t="shared" si="2"/>
         <v>0.03</v>
       </c>
-      <c r="K11" s="37"/>
+      <c r="K11" s="38"/>
       <c r="L11" s="12">
         <v>0.3</v>
       </c>
@@ -5905,7 +5944,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="37"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="12">
         <v>0.5</v>
       </c>
@@ -5933,7 +5972,7 @@
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
-      <c r="K12" s="37"/>
+      <c r="K12" s="38"/>
       <c r="L12" s="12">
         <v>0.5</v>
       </c>
@@ -5963,7 +6002,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="37"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="12">
         <v>1</v>
       </c>
@@ -5991,7 +6030,7 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="K13" s="37"/>
+      <c r="K13" s="38"/>
       <c r="L13" s="12">
         <v>1</v>
       </c>
@@ -6171,24 +6210,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
@@ -6247,28 +6286,28 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="33" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="33" t="s">
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="34"/>
-      <c r="P3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="36"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -6335,10 +6374,10 @@
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="21" t="s">
+      <c r="R6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="21"/>
+      <c r="S6" s="23"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -6376,10 +6415,10 @@
       <c r="Q7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R7" s="38" t="s">
+      <c r="R7" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="S7" s="38"/>
+      <c r="S7" s="39"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
@@ -6390,18 +6429,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21" t="s">
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
@@ -6415,18 +6454,18 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="21">
+      <c r="I9" s="23">
         <v>17</v>
       </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21">
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23">
         <v>4</v>
       </c>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
@@ -6445,11 +6484,11 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="21" t="s">
+      <c r="N10" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -6468,24 +6507,18 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="22">
+      <c r="N11" s="24">
         <f>100/(2^3-1)*N9</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I6:P6"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="I8:M8"/>
@@ -6493,6 +6526,12 @@
     <mergeCell ref="I9:M9"/>
     <mergeCell ref="N9:P9"/>
     <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="I6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>